<commit_message>
started work on form maps; changed view and controller to allow multiple templates per route
</commit_message>
<xml_diff>
--- a/doc/design.xlsx
+++ b/doc/design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="client_server" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,8 @@
     <sheet name="references" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="model" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="buttons" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="form" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="controller" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="264">
   <si>
     <t>client</t>
   </si>
@@ -704,6 +706,120 @@
   <si>
     <t>snippet for registering event handler</t>
   </si>
+  <si>
+    <t>atom type</t>
+  </si>
+  <si>
+    <t>form label</t>
+  </si>
+  <si>
+    <t>form input</t>
+  </si>
+  <si>
+    <t>placeholder</t>
+  </si>
+  <si>
+    <t>label.class=radio-inline</t>
+  </si>
+  <si>
+    <t>input.type=radio</t>
+  </si>
+  <si>
+    <t>label.class=form-control</t>
+  </si>
+  <si>
+    <t>input.type=date</t>
+  </si>
+  <si>
+    <t>dd.mm.jjjj</t>
+  </si>
+  <si>
+    <t>input.type=datetime</t>
+  </si>
+  <si>
+    <t>dd.mm.jjjj uu:mm:ss</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>input.type=number</t>
+  </si>
+  <si>
+    <t>123.45</t>
+  </si>
+  <si>
+    <t>memo</t>
+  </si>
+  <si>
+    <t>textarea.rows.cols</t>
+  </si>
+  <si>
+    <t>input.type=text</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>input.type=time</t>
+  </si>
+  <si>
+    <t>uu:mm:ss</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>input.type=url</t>
+  </si>
+  <si>
+    <t>enumeration type</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>page mode</t>
+  </si>
+  <si>
+    <t>fragment mode</t>
+  </si>
+  <si>
+    <t>xml mode</t>
+  </si>
+  <si>
+    <t>json mode</t>
+  </si>
+  <si>
+    <t>serialize</t>
+  </si>
+  <si>
+    <t>render with template given by render tree</t>
+  </si>
+  <si>
+    <t>convert to XML</t>
+  </si>
+  <si>
+    <t>encode_dict / json.dumps</t>
+  </si>
+  <si>
+    <t>finalize</t>
+  </si>
+  <si>
+    <t>render with site template</t>
+  </si>
 </sst>
 </file>
 
@@ -908,7 +1024,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1061,6 +1177,18 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1138,15 +1266,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>113760</xdr:colOff>
+      <xdr:colOff>167760</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>68040</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>124920</xdr:colOff>
+      <xdr:colOff>178920</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>72720</xdr:rowOff>
+      <xdr:rowOff>54720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1155,8 +1283,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2323440" y="1368360"/>
-          <a:ext cx="2077920" cy="4680"/>
+          <a:off x="2377440" y="1350360"/>
+          <a:ext cx="2097000" cy="4680"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1181,15 +1309,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>135360</xdr:colOff>
+      <xdr:colOff>189360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>107640</xdr:rowOff>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>124920</xdr:colOff>
+      <xdr:colOff>178920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>90000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1198,8 +1326,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2345040" y="595080"/>
-          <a:ext cx="2056320" cy="360"/>
+          <a:off x="2399040" y="577080"/>
+          <a:ext cx="2075400" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1224,15 +1352,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>127440</xdr:colOff>
+      <xdr:colOff>181440</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>39600</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>129960</xdr:colOff>
+      <xdr:colOff>183960</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>22680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1241,8 +1369,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5375520" y="1177200"/>
-          <a:ext cx="1821960" cy="1080"/>
+          <a:off x="5448600" y="1159200"/>
+          <a:ext cx="1840680" cy="1080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1267,15 +1395,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>129240</xdr:colOff>
+      <xdr:colOff>183240</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>93960</xdr:rowOff>
+      <xdr:rowOff>75960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>124920</xdr:colOff>
+      <xdr:colOff>178920</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1284,8 +1412,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2338920" y="2694600"/>
-          <a:ext cx="2062440" cy="1080"/>
+          <a:off x="2392920" y="2676600"/>
+          <a:ext cx="2081520" cy="1080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1310,15 +1438,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>133560</xdr:colOff>
+      <xdr:colOff>187560</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>135360</xdr:rowOff>
+      <xdr:rowOff>117360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>129960</xdr:colOff>
+      <xdr:colOff>183960</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>135720</xdr:rowOff>
+      <xdr:rowOff>117720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1327,8 +1455,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5381640" y="785520"/>
-          <a:ext cx="1815840" cy="360"/>
+          <a:off x="5454720" y="767520"/>
+          <a:ext cx="1834560" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1353,15 +1481,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>132480</xdr:colOff>
+      <xdr:colOff>186480</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>124920</xdr:colOff>
+      <xdr:colOff>178920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>33120</xdr:rowOff>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1370,8 +1498,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2342160" y="2304720"/>
-          <a:ext cx="2059200" cy="3960"/>
+          <a:off x="2396160" y="2286720"/>
+          <a:ext cx="2078280" cy="3960"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1396,15 +1524,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>129960</xdr:colOff>
+      <xdr:colOff>183960</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>128520</xdr:rowOff>
+      <xdr:rowOff>110520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>124920</xdr:colOff>
+      <xdr:colOff>178920</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>129960</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1413,8 +1541,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2339640" y="3054600"/>
-          <a:ext cx="2061720" cy="1440"/>
+          <a:off x="2393640" y="3036600"/>
+          <a:ext cx="2080800" cy="1440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1439,15 +1567,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>141840</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:colOff>195840</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>140400</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:colOff>194400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1456,8 +1584,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5389920" y="3261240"/>
-          <a:ext cx="1818000" cy="0"/>
+          <a:off x="5463000" y="3243240"/>
+          <a:ext cx="1836720" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1482,15 +1610,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>149760</xdr:colOff>
+      <xdr:colOff>203760</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>55440</xdr:rowOff>
+      <xdr:rowOff>37440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>135360</xdr:colOff>
+      <xdr:colOff>189360</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>56160</xdr:rowOff>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1499,8 +1627,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5397840" y="3631680"/>
-          <a:ext cx="1805040" cy="720"/>
+          <a:off x="5470920" y="3613680"/>
+          <a:ext cx="1823760" cy="720"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1525,15 +1653,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>126000</xdr:colOff>
+      <xdr:colOff>180000</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>76680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>119880</xdr:colOff>
+      <xdr:colOff>173880</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>99000</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1542,8 +1670,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2335680" y="3833280"/>
-          <a:ext cx="2060640" cy="4320"/>
+          <a:off x="2389680" y="3815280"/>
+          <a:ext cx="2079720" cy="4320"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1568,15 +1696,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>667440</xdr:colOff>
+      <xdr:colOff>721440</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>672480</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:colOff>726480</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1585,7 +1713,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="1657800" y="4689720"/>
+          <a:off x="1711800" y="4671720"/>
           <a:ext cx="5040" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1611,15 +1739,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>109800</xdr:colOff>
+      <xdr:colOff>163800</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>776520</xdr:colOff>
+      <xdr:colOff>830520</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>20520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1628,7 +1756,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2319480" y="4590000"/>
+          <a:off x="2373480" y="4572000"/>
           <a:ext cx="666720" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1654,15 +1782,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>140760</xdr:colOff>
+      <xdr:colOff>194760</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>126000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>777240</xdr:colOff>
+      <xdr:colOff>831240</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1671,7 +1799,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2350440" y="5345640"/>
+          <a:off x="2404440" y="5327640"/>
           <a:ext cx="636480" cy="360"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1696,15 +1824,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>770400</xdr:colOff>
+      <xdr:colOff>824400</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:rowOff>30600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>770400</xdr:colOff>
+      <xdr:colOff>824400</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1713,7 +1841,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2980080" y="4600080"/>
+          <a:off x="3034080" y="4582080"/>
           <a:ext cx="0" cy="751680"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1738,15 +1866,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>130680</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:colOff>184680</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>125280</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:colOff>179280</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1755,8 +1883,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2340360" y="5537160"/>
-          <a:ext cx="2061360" cy="0"/>
+          <a:off x="2394360" y="5519160"/>
+          <a:ext cx="2080440" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1781,15 +1909,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>146160</xdr:colOff>
+      <xdr:colOff>200160</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>135360</xdr:colOff>
+      <xdr:colOff>189360</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>25560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1798,8 +1926,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5394240" y="5727240"/>
-          <a:ext cx="1808640" cy="5760"/>
+          <a:off x="5467320" y="5709240"/>
+          <a:ext cx="1827360" cy="5760"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1824,15 +1952,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>134280</xdr:colOff>
+      <xdr:colOff>188280</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>124920</xdr:colOff>
+      <xdr:colOff>178920</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>109800</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1841,8 +1969,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5382360" y="6118560"/>
-          <a:ext cx="1810080" cy="5760"/>
+          <a:off x="5455440" y="6100560"/>
+          <a:ext cx="1828800" cy="5760"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1867,15 +1995,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>145800</xdr:colOff>
+      <xdr:colOff>199800</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>126360</xdr:rowOff>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>124920</xdr:colOff>
+      <xdr:colOff>178920</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>127080</xdr:rowOff>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1884,8 +2012,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2355480" y="6303600"/>
-          <a:ext cx="2045880" cy="720"/>
+          <a:off x="2409480" y="6285600"/>
+          <a:ext cx="2064960" cy="720"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1920,18 +2048,18 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="1" sqref="C6 A7"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="9" min="6" style="1" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -28751,17 +28879,17 @@
   </sheetPr>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.8137651821862"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -29102,23 +29230,23 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="C6 B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.1740890688259"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -29416,17 +29544,17 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="C6 C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1023" min="9" style="1" width="9.10526315789474"/>
@@ -29680,21 +29808,21 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="1" sqref="C6 F23"/>
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="1" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="1.60728744939271"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="20" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="1.39271255060729"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.81781376518219"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="1.60728744939271"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="1.39271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="20" width="7.71255060728745"/>
-    <col collapsed="false" hidden="false" max="15" min="12" style="2" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="2" width="9.96356275303644"/>
     <col collapsed="false" hidden="false" max="20" min="16" style="1" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="1" width="9.10526315789474"/>
   </cols>
@@ -30550,7 +30678,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="1" sqref="C6 H20"/>
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -30563,8 +30691,8 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="8" style="1" width="5.67611336032389"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="9.96356275303644"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31027,4 +31155,414 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Standaard"&amp;12Pagina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.21457489878543"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.39271255060729"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F6" s="38" t="n">
+        <v>123</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standaard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standaard"&amp;12Pagina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.21457489878543"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="16.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="39"/>
+      <c r="B1" s="40" t="s">
+        <v>254</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="25.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="24.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="40" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Standaard"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standaard"&amp;12Pagina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added foundation for I18N, added Button class
</commit_message>
<xml_diff>
--- a/doc/design.xlsx
+++ b/doc/design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="render_tree" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="422">
   <si>
     <t xml:space="preserve">component</t>
   </si>
@@ -743,67 +743,174 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">comment</t>
+    <t xml:space="preserve">param</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ptype</t>
   </si>
   <si>
     <t xml:space="preserve">panel</t>
   </si>
   <si>
-    <t xml:space="preserve">enabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">button type=button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">btn-default enabled</t>
-  </si>
-  <si>
     <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">no</t>
   </si>
   <si>
-    <t xml:space="preserve">disabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">btn-default disabled</t>
-  </si>
-  <si>
     <t xml:space="preserve">toggle, prompt</t>
   </si>
   <si>
-    <t xml:space="preserve">JS availability is undetectable!</t>
-  </si>
-  <si>
     <t xml:space="preserve">form</t>
   </si>
   <si>
-    <t xml:space="preserve">button type=submit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not used in practice</t>
-  </si>
-  <si>
     <t xml:space="preserve">grid</t>
   </si>
   <si>
-    <t xml:space="preserve">btn-sm enabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">btn-sm disabled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">page top hook</t>
-  </si>
-  <si>
-    <t xml:space="preserve">include bootbox.js</t>
-  </si>
-  <si>
-    <t xml:space="preserve">page bottom hook</t>
-  </si>
-  <si>
-    <t xml:space="preserve">snippet for registering event handler</t>
+    <t xml:space="preserve">depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diepte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/person/{id}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;none&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FFF58220"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/person</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFF58220"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/123456</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">fa-book-open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTML:a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">href</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data-method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data-bind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTML:button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn btn-primary btn-sm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fa-trash-alt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btn btn-light btn-xs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/person/fetch?pid={pid}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fetch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fa-hand-point-right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?????????</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre-submit prompting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/person/123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fa-check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTML:form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre-submit validation???</t>
   </si>
   <si>
     <t xml:space="preserve">domain</t>
@@ -848,9 +955,6 @@
     <t xml:space="preserve">Getal</t>
   </si>
   <si>
-    <t xml:space="preserve">number</t>
-  </si>
-  <si>
     <t xml:space="preserve">Leeftijd</t>
   </si>
   <si>
@@ -1109,9 +1213,6 @@
     <t xml:space="preserve">render with site template</t>
   </si>
   <si>
-    <t xml:space="preserve">route</t>
-  </si>
-  <si>
     <t xml:space="preserve">bool enum date time</t>
   </si>
   <si>
@@ -1122,9 +1223,6 @@
   </si>
   <si>
     <t xml:space="preserve">itemref</t>
-  </si>
-  <si>
-    <t xml:space="preserve">depth</t>
   </si>
   <si>
     <t xml:space="preserve">show item</t>
@@ -1229,7 +1327,7 @@
     <numFmt numFmtId="165" formatCode="YYYY/DD/MM"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY\ HH:MM"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1443,6 +1541,21 @@
       <charset val="1"/>
     </font>
     <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FFF58220"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFF58220"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FFDD4814"/>
@@ -1509,7 +1622,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1519,25 +1632,49 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFFFE5CA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFBCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFE0EFD4"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99CCFF"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFE0EFD4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFFE5CA"/>
+        <bgColor rgb="FFFFFBCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAA61A"/>
+        <bgColor rgb="FFF58220"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFBCC"/>
+        <bgColor rgb="FFFFE5CA"/>
       </patternFill>
     </fill>
   </fills>
@@ -1599,7 +1736,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="89">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1808,10 +1945,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1820,11 +1953,75 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1836,18 +2033,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1856,7 +2041,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1868,15 +2073,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1900,7 +2105,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFFE5CA"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -1917,12 +2122,12 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFFBCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF6633"/>
+      <rgbColor rgb="FFF58220"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1933,17 +2138,17 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFE0EFD4"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFF6633"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF0047FF"/>
       <rgbColor rgb="FF33CC66"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFAA61A"/>
       <rgbColor rgb="FFE46C0A"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF999999"/>
@@ -30908,26 +31113,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="66" t="s">
-        <v>359</v>
+      <c r="A1" s="83" t="s">
+        <v>249</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>360</v>
+        <v>387</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>361</v>
+        <v>388</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>362</v>
-      </c>
-      <c r="E1" s="66" t="s">
-        <v>363</v>
-      </c>
-      <c r="F1" s="66" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1" s="83" t="s">
+        <v>390</v>
+      </c>
+      <c r="F1" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="66" t="s">
-        <v>364</v>
+      <c r="G1" s="83" t="s">
+        <v>246</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -30938,25 +31143,25 @@
       <c r="N1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="65" t="s">
-        <v>365</v>
-      </c>
-      <c r="B2" s="65" t="s">
-        <v>366</v>
-      </c>
-      <c r="C2" s="65" t="s">
-        <v>366</v>
-      </c>
-      <c r="D2" s="65" t="s">
-        <v>366</v>
-      </c>
-      <c r="E2" s="65" t="s">
-        <v>366</v>
-      </c>
-      <c r="F2" s="65" t="s">
-        <v>367</v>
-      </c>
-      <c r="G2" s="65" t="n">
+      <c r="A2" s="82" t="s">
+        <v>391</v>
+      </c>
+      <c r="B2" s="82" t="s">
+        <v>392</v>
+      </c>
+      <c r="C2" s="82" t="s">
+        <v>392</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>392</v>
+      </c>
+      <c r="E2" s="82" t="s">
+        <v>392</v>
+      </c>
+      <c r="F2" s="82" t="s">
+        <v>393</v>
+      </c>
+      <c r="G2" s="82" t="n">
         <v>2</v>
       </c>
       <c r="H2" s="3"/>
@@ -30968,25 +31173,25 @@
       <c r="N2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="65" t="s">
-        <v>368</v>
-      </c>
-      <c r="B3" s="65" t="s">
-        <v>366</v>
-      </c>
-      <c r="C3" s="65" t="s">
-        <v>366</v>
-      </c>
-      <c r="D3" s="65" t="s">
-        <v>366</v>
-      </c>
-      <c r="E3" s="65" t="s">
-        <v>369</v>
-      </c>
-      <c r="F3" s="65" t="s">
-        <v>370</v>
-      </c>
-      <c r="G3" s="65" t="n">
+      <c r="A3" s="82" t="s">
+        <v>394</v>
+      </c>
+      <c r="B3" s="82" t="s">
+        <v>392</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>392</v>
+      </c>
+      <c r="D3" s="82" t="s">
+        <v>392</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>395</v>
+      </c>
+      <c r="F3" s="82" t="s">
+        <v>396</v>
+      </c>
+      <c r="G3" s="82" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="3"/>
@@ -30998,25 +31203,25 @@
       <c r="N3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="65" t="s">
-        <v>371</v>
-      </c>
-      <c r="B4" s="65" t="s">
-        <v>366</v>
-      </c>
-      <c r="C4" s="65" t="s">
-        <v>366</v>
-      </c>
-      <c r="D4" s="65" t="s">
-        <v>372</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>372</v>
-      </c>
-      <c r="F4" s="65" t="s">
-        <v>372</v>
-      </c>
-      <c r="G4" s="65" t="n">
+      <c r="A4" s="82" t="s">
+        <v>397</v>
+      </c>
+      <c r="B4" s="82" t="s">
+        <v>392</v>
+      </c>
+      <c r="C4" s="82" t="s">
+        <v>392</v>
+      </c>
+      <c r="D4" s="82" t="s">
+        <v>398</v>
+      </c>
+      <c r="E4" s="82" t="s">
+        <v>398</v>
+      </c>
+      <c r="F4" s="82" t="s">
+        <v>398</v>
+      </c>
+      <c r="G4" s="82" t="n">
         <v>1</v>
       </c>
       <c r="H4" s="3"/>
@@ -31044,17 +31249,17 @@
       <c r="N5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="68" t="s">
-        <v>373</v>
-      </c>
-      <c r="B6" s="69" t="s">
-        <v>374</v>
-      </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
+      <c r="A6" s="85" t="s">
+        <v>399</v>
+      </c>
+      <c r="B6" s="86" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -31064,17 +31269,17 @@
       <c r="N6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="68" t="s">
-        <v>375</v>
-      </c>
-      <c r="B7" s="69" t="s">
-        <v>376</v>
-      </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
+      <c r="A7" s="85" t="s">
+        <v>401</v>
+      </c>
+      <c r="B7" s="86" t="s">
+        <v>402</v>
+      </c>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -31084,17 +31289,17 @@
       <c r="N7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="68" t="s">
-        <v>377</v>
-      </c>
-      <c r="B8" s="69" t="s">
-        <v>378</v>
-      </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
+      <c r="A8" s="85" t="s">
+        <v>403</v>
+      </c>
+      <c r="B8" s="86" t="s">
+        <v>404</v>
+      </c>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -31158,13 +31363,13 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>380</v>
-      </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
+        <v>405</v>
+      </c>
+      <c r="C1" s="87" t="s">
+        <v>406</v>
+      </c>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
       <c r="F1" s="3"/>
       <c r="G1" s="4" t="s">
         <v>170</v>
@@ -31176,13 +31381,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>381</v>
+        <v>407</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>383</v>
+        <v>409</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>58</v>
@@ -31200,10 +31405,10 @@
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>384</v>
+        <v>410</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>383</v>
+        <v>409</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>62</v>
@@ -31221,10 +31426,10 @@
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>385</v>
+        <v>411</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>383</v>
+        <v>409</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>64</v>
@@ -31234,7 +31439,7 @@
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="28" t="s">
-        <v>386</v>
+        <v>412</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -31257,13 +31462,13 @@
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="C6" s="71" t="s">
+        <v>405</v>
+      </c>
+      <c r="C6" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
       <c r="F6" s="3"/>
       <c r="G6" s="4" t="s">
         <v>170</v>
@@ -31278,7 +31483,7 @@
         <v>153</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>58</v>
@@ -31297,7 +31502,7 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>384</v>
+        <v>410</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>62</v>
@@ -31316,16 +31521,16 @@
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>388</v>
+        <v>414</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="28" t="s">
-        <v>389</v>
+        <v>415</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -31336,10 +31541,10 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>390</v>
+        <v>416</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>391</v>
+        <v>417</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -31355,10 +31560,10 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>392</v>
+        <v>418</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>393</v>
+        <v>419</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -31374,7 +31579,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>394</v>
+        <v>420</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -31401,13 +31606,13 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="C14" s="70" t="s">
-        <v>380</v>
-      </c>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
+        <v>405</v>
+      </c>
+      <c r="C14" s="87" t="s">
+        <v>406</v>
+      </c>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
       <c r="F14" s="3"/>
       <c r="G14" s="4" t="s">
         <v>170</v>
@@ -31419,13 +31624,13 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>381</v>
+        <v>407</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>383</v>
+        <v>409</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>58</v>
@@ -31443,10 +31648,10 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>384</v>
+        <v>410</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>383</v>
+        <v>409</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>62</v>
@@ -31464,10 +31669,10 @@
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>385</v>
+        <v>411</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>395</v>
+        <v>421</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>64</v>
@@ -31477,7 +31682,7 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="28" t="s">
-        <v>386</v>
+        <v>412</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -31500,13 +31705,13 @@
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="C19" s="71" t="s">
+        <v>405</v>
+      </c>
+      <c r="C19" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="88"/>
       <c r="F19" s="3"/>
       <c r="G19" s="4" t="s">
         <v>170</v>
@@ -31521,7 +31726,7 @@
         <v>153</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>58</v>
@@ -31540,7 +31745,7 @@
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>384</v>
+        <v>410</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>62</v>
@@ -31559,16 +31764,16 @@
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>388</v>
+        <v>414</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="28" t="s">
-        <v>389</v>
+        <v>415</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -31579,10 +31784,10 @@
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>390</v>
+        <v>416</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>391</v>
+        <v>417</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -31598,10 +31803,10 @@
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>392</v>
+        <v>418</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>393</v>
+        <v>419</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -31617,7 +31822,7 @@
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>394</v>
+        <v>420</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -31661,7 +31866,7 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -33864,24 +34069,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M22" activeCellId="0" sqref="M22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E64" activeCellId="0" sqref="E64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="1" width="5.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="35.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="5.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="12.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="1" width="10.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -33900,466 +34112,1368 @@
       <c r="E1" s="48" t="s">
         <v>232</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="48"/>
+      <c r="G1" s="48" t="s">
         <v>233</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="H1" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="I1" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="J1" s="49" t="s">
         <v>234</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="K1" s="49" t="s">
         <v>235</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="L1" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="M1" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="N1" s="49" t="s">
         <v>237</v>
       </c>
+      <c r="O1" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="P1" s="49" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q1" s="50"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="50" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C2" s="50"/>
-      <c r="D2" s="50" t="s">
-        <v>239</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="F2" s="50" t="s">
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="51" t="s">
         <v>241</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="51" t="s">
+      <c r="J2" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="K2" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="L2" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="M2" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="J2" s="51" t="s">
-        <v>242</v>
-      </c>
-      <c r="K2" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="L2" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="M2" s="50"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="50"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="50" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C3" s="50"/>
-      <c r="D3" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="F3" s="50" t="s">
-        <v>245</v>
-      </c>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
       <c r="G3" s="50"/>
-      <c r="H3" s="51" t="s">
+      <c r="H3" s="50"/>
+      <c r="I3" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="J3" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="K3" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="L3" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="I3" s="51" t="s">
+      <c r="M3" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="J3" s="51" t="s">
-        <v>242</v>
-      </c>
-      <c r="K3" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="L3" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="M3" s="50"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="50"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="50" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C4" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="50" t="s">
-        <v>239</v>
-      </c>
-      <c r="E4" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="F4" s="50" t="s">
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="I4" s="51" t="s">
         <v>241</v>
       </c>
-      <c r="G4" s="50" t="s">
-        <v>246</v>
-      </c>
-      <c r="H4" s="51" t="s">
+      <c r="J4" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="K4" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="L4" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="I4" s="51" t="s">
+      <c r="M4" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="J4" s="51" t="s">
-        <v>242</v>
-      </c>
-      <c r="K4" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="L4" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="M4" s="52" t="s">
-        <v>247</v>
-      </c>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="50"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="50" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C5" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="E5" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="F5" s="50" t="s">
-        <v>245</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>246</v>
-      </c>
-      <c r="H5" s="51" t="s">
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="I5" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="J5" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="K5" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="L5" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="I5" s="51" t="s">
+      <c r="M5" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="J5" s="51" t="s">
-        <v>242</v>
-      </c>
-      <c r="K5" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="L5" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="M5" s="3"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="50" t="s">
         <v>45</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C6" s="50"/>
-      <c r="D6" s="50" t="s">
-        <v>239</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>249</v>
-      </c>
-      <c r="F6" s="50" t="s">
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51" t="s">
         <v>241</v>
       </c>
-      <c r="G6" s="50"/>
-      <c r="H6" s="51" t="s">
-        <v>242</v>
-      </c>
-      <c r="I6" s="51" t="s">
-        <v>242</v>
-      </c>
       <c r="J6" s="51" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K6" s="51" t="s">
         <v>242</v>
       </c>
       <c r="L6" s="51" t="s">
-        <v>242</v>
-      </c>
-      <c r="M6" s="50"/>
+        <v>241</v>
+      </c>
+      <c r="M6" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="51"/>
+      <c r="Q6" s="50"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="53" t="s">
-        <v>248</v>
-      </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53" t="s">
+      <c r="B7" s="52" t="s">
         <v>244</v>
       </c>
-      <c r="E7" s="53" t="s">
-        <v>249</v>
-      </c>
-      <c r="F7" s="53" t="s">
-        <v>245</v>
-      </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="54" t="s">
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53" t="s">
+        <v>241</v>
+      </c>
+      <c r="J7" s="53" t="s">
+        <v>241</v>
+      </c>
+      <c r="K7" s="53" t="s">
         <v>242</v>
       </c>
-      <c r="I7" s="54" t="s">
-        <v>242</v>
-      </c>
-      <c r="J7" s="54" t="s">
-        <v>243</v>
-      </c>
-      <c r="K7" s="54" t="s">
-        <v>242</v>
-      </c>
-      <c r="L7" s="54" t="s">
-        <v>242</v>
+      <c r="L7" s="53" t="s">
+        <v>241</v>
       </c>
       <c r="M7" s="53" t="s">
-        <v>250</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="52"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="50" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C8" s="50"/>
-      <c r="D8" s="50" t="s">
-        <v>239</v>
-      </c>
-      <c r="E8" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="F8" s="50" t="s">
-        <v>252</v>
-      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
       <c r="G8" s="50"/>
-      <c r="H8" s="51" t="s">
-        <v>243</v>
-      </c>
+      <c r="H8" s="50"/>
       <c r="I8" s="51" t="s">
         <v>242</v>
       </c>
       <c r="J8" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="K8" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="L8" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="K8" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="L8" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="M8" s="50"/>
+      <c r="M8" s="51" t="s">
+        <v>242</v>
+      </c>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="50"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="50" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C9" s="50"/>
-      <c r="D9" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="F9" s="50" t="s">
-        <v>253</v>
-      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
       <c r="G9" s="50"/>
-      <c r="H9" s="51" t="s">
-        <v>243</v>
-      </c>
+      <c r="H9" s="50"/>
       <c r="I9" s="51" t="s">
         <v>242</v>
       </c>
       <c r="J9" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="K9" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="L9" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="K9" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="L9" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="M9" s="50"/>
+      <c r="M9" s="51" t="s">
+        <v>242</v>
+      </c>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="50"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="50" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C10" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="D10" s="50" t="s">
-        <v>239</v>
-      </c>
-      <c r="E10" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="F10" s="50" t="s">
-        <v>252</v>
-      </c>
-      <c r="G10" s="50" t="s">
-        <v>246</v>
-      </c>
-      <c r="H10" s="51" t="s">
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50" t="s">
         <v>243</v>
       </c>
       <c r="I10" s="51" t="s">
         <v>242</v>
       </c>
       <c r="J10" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="K10" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="L10" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="K10" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="L10" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="M10" s="50"/>
+      <c r="M10" s="51" t="s">
+        <v>242</v>
+      </c>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="50"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="50" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C11" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="D11" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="E11" s="50" t="s">
-        <v>240</v>
-      </c>
-      <c r="F11" s="50" t="s">
-        <v>253</v>
-      </c>
-      <c r="G11" s="50" t="s">
-        <v>246</v>
-      </c>
-      <c r="H11" s="51" t="s">
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50" t="s">
         <v>243</v>
       </c>
       <c r="I11" s="51" t="s">
         <v>242</v>
       </c>
       <c r="J11" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="K11" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="L11" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="K11" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="L11" s="51" t="s">
-        <v>243</v>
-      </c>
-      <c r="M11" s="50"/>
+      <c r="M11" s="51" t="s">
+        <v>242</v>
+      </c>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="50"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51" t="s">
+        <v>246</v>
+      </c>
+      <c r="O12" s="51" t="s">
+        <v>247</v>
+      </c>
+      <c r="P12" s="51" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q12" s="50"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C13" s="3" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="54" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>250</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>251</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="F13" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54" t="s">
+        <v>237</v>
+      </c>
+      <c r="I13" s="54" t="s">
+        <v>238</v>
+      </c>
+      <c r="J13" s="54" t="s">
+        <v>239</v>
+      </c>
+      <c r="K13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="55"/>
+      <c r="B14" s="56" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="I14" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="J14" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="K14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="55"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>251</v>
+      </c>
+      <c r="E16" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="F16" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="54" t="s">
+        <v>236</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>237</v>
+      </c>
+      <c r="I16" s="54" t="s">
+        <v>238</v>
+      </c>
+      <c r="J16" s="54" t="s">
+        <v>239</v>
+      </c>
+      <c r="K16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="55"/>
+      <c r="B17" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56" t="s">
+        <v>256</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>257</v>
+      </c>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="55"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="54" t="s">
+        <v>258</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>260</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>261</v>
+      </c>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="56"/>
+      <c r="B20" s="57" t="s">
+        <v>255</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>253</v>
+      </c>
+      <c r="D20" s="56" t="s">
+        <v>262</v>
+      </c>
+      <c r="E20" s="55"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="56"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="56"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="54" t="s">
+        <v>263</v>
+      </c>
+      <c r="B22" s="56"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="F22" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="56"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56" t="s">
+        <v>264</v>
+      </c>
+      <c r="E23" s="56" t="s">
+        <v>256</v>
+      </c>
+      <c r="F23" s="56" t="s">
+        <v>257</v>
+      </c>
+      <c r="G23" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="B26" s="58" t="s">
+        <v>250</v>
+      </c>
+      <c r="C26" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="E26" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="F26" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58" t="s">
+        <v>237</v>
+      </c>
+      <c r="I26" s="58" t="s">
+        <v>238</v>
+      </c>
+      <c r="J26" s="58" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="59"/>
+      <c r="B27" s="60" t="s">
+        <v>252</v>
+      </c>
+      <c r="C27" s="60" t="s">
+        <v>265</v>
+      </c>
+      <c r="D27" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="E27" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60" t="s">
         <v>254</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3" t="s">
+      <c r="I27" s="60" t="s">
+        <v>254</v>
+      </c>
+      <c r="J27" s="60" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="59"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="58" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="E29" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="F29" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="58" t="s">
+        <v>236</v>
+      </c>
+      <c r="H29" s="58" t="s">
+        <v>237</v>
+      </c>
+      <c r="I29" s="58" t="s">
+        <v>238</v>
+      </c>
+      <c r="J29" s="58" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="59"/>
+      <c r="B30" s="61" t="s">
         <v>255</v>
       </c>
+      <c r="C30" s="60" t="s">
+        <v>265</v>
+      </c>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60" t="s">
+        <v>266</v>
+      </c>
+      <c r="F30" s="60" t="s">
+        <v>267</v>
+      </c>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60" t="s">
+        <v>254</v>
+      </c>
+      <c r="I30" s="60" t="s">
+        <v>254</v>
+      </c>
+      <c r="J30" s="60" t="s">
+        <v>254</v>
+      </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3" t="s">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="59"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="58" t="s">
+        <v>258</v>
+      </c>
+      <c r="B32" s="58" t="s">
+        <v>259</v>
+      </c>
+      <c r="C32" s="58" t="s">
+        <v>260</v>
+      </c>
+      <c r="D32" s="58" t="s">
+        <v>261</v>
+      </c>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+    </row>
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="60"/>
+      <c r="B33" s="61" t="s">
+        <v>255</v>
+      </c>
+      <c r="C33" s="60" t="s">
+        <v>265</v>
+      </c>
+      <c r="D33" s="60" t="s">
+        <v>268</v>
+      </c>
+      <c r="E33" s="59"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="60"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="58" t="s">
+        <v>263</v>
+      </c>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="F35" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="60"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="60" t="s">
+        <v>269</v>
+      </c>
+      <c r="E36" s="60" t="s">
+        <v>266</v>
+      </c>
+      <c r="F36" s="60" t="s">
+        <v>267</v>
+      </c>
+      <c r="G36" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="H36" s="60"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="60"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="62" t="s">
+        <v>249</v>
+      </c>
+      <c r="B39" s="62" t="s">
+        <v>250</v>
+      </c>
+      <c r="C39" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="62" t="s">
+        <v>251</v>
+      </c>
+      <c r="E39" s="62" t="s">
+        <v>234</v>
+      </c>
+      <c r="F39" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="G39" s="62"/>
+      <c r="H39" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="I39" s="62" t="s">
+        <v>238</v>
+      </c>
+      <c r="J39" s="62" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="63"/>
+      <c r="B40" s="64" t="s">
+        <v>270</v>
+      </c>
+      <c r="C40" s="64" t="s">
+        <v>253</v>
+      </c>
+      <c r="D40" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" s="64" t="s">
+        <v>271</v>
+      </c>
+      <c r="F40" s="64" t="s">
         <v>257</v>
       </c>
+      <c r="G40" s="64"/>
+      <c r="H40" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="I40" s="64" t="s">
+        <v>272</v>
+      </c>
+      <c r="J40" s="64" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="63"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="64"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="64"/>
+      <c r="H41" s="64"/>
+      <c r="I41" s="64"/>
+      <c r="J41" s="64"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="62" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="62" t="s">
+        <v>251</v>
+      </c>
+      <c r="E42" s="62" t="s">
+        <v>234</v>
+      </c>
+      <c r="F42" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="G42" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="H42" s="62" t="s">
+        <v>237</v>
+      </c>
+      <c r="I42" s="62" t="s">
+        <v>238</v>
+      </c>
+      <c r="J42" s="62" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="63"/>
+      <c r="B43" s="65" t="s">
+        <v>270</v>
+      </c>
+      <c r="C43" s="64" t="s">
+        <v>253</v>
+      </c>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64" t="s">
+        <v>273</v>
+      </c>
+      <c r="F43" s="64" t="s">
+        <v>274</v>
+      </c>
+      <c r="G43" s="64"/>
+      <c r="H43" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="I43" s="64" t="s">
+        <v>272</v>
+      </c>
+      <c r="J43" s="64" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="63"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="64"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="62" t="s">
+        <v>275</v>
+      </c>
+      <c r="B45" s="62" t="s">
+        <v>259</v>
+      </c>
+      <c r="C45" s="62" t="s">
+        <v>260</v>
+      </c>
+      <c r="D45" s="62" t="s">
+        <v>261</v>
+      </c>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="63"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="64"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="64"/>
+      <c r="B46" s="65" t="s">
+        <v>270</v>
+      </c>
+      <c r="C46" s="64" t="s">
+        <v>253</v>
+      </c>
+      <c r="D46" s="66" t="s">
+        <v>276</v>
+      </c>
+      <c r="E46" s="63"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="64"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="64"/>
+      <c r="J46" s="64"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="64"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="64"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="64"/>
+      <c r="J47" s="64"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="62" t="s">
+        <v>263</v>
+      </c>
+      <c r="B48" s="64"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="E48" s="62" t="s">
+        <v>234</v>
+      </c>
+      <c r="F48" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="G48" s="62" t="s">
+        <v>170</v>
+      </c>
+      <c r="H48" s="64"/>
+      <c r="I48" s="64"/>
+      <c r="J48" s="64"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="64"/>
+      <c r="B49" s="64"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="64" t="s">
+        <v>264</v>
+      </c>
+      <c r="E49" s="64" t="s">
+        <v>273</v>
+      </c>
+      <c r="F49" s="64" t="s">
+        <v>274</v>
+      </c>
+      <c r="G49" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="H49" s="64"/>
+      <c r="I49" s="64"/>
+      <c r="J49" s="64"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="65" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="67" t="s">
+        <v>249</v>
+      </c>
+      <c r="B52" s="67" t="s">
+        <v>250</v>
+      </c>
+      <c r="C52" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="67" t="s">
+        <v>251</v>
+      </c>
+      <c r="E52" s="67" t="s">
+        <v>234</v>
+      </c>
+      <c r="F52" s="67" t="s">
+        <v>51</v>
+      </c>
+      <c r="G52" s="67"/>
+      <c r="H52" s="67" t="s">
+        <v>237</v>
+      </c>
+      <c r="I52" s="67" t="s">
+        <v>238</v>
+      </c>
+      <c r="J52" s="67" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="68"/>
+      <c r="B53" s="69" t="s">
+        <v>252</v>
+      </c>
+      <c r="C53" s="70" t="s">
+        <v>278</v>
+      </c>
+      <c r="D53" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" s="70" t="s">
+        <v>279</v>
+      </c>
+      <c r="F53" s="70" t="s">
+        <v>279</v>
+      </c>
+      <c r="G53" s="70"/>
+      <c r="H53" s="60" t="s">
+        <v>254</v>
+      </c>
+      <c r="I53" s="60" t="s">
+        <v>254</v>
+      </c>
+      <c r="J53" s="60" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="68"/>
+      <c r="B54" s="68"/>
+      <c r="C54" s="70"/>
+      <c r="D54" s="70"/>
+      <c r="E54" s="70"/>
+      <c r="F54" s="70"/>
+      <c r="G54" s="70"/>
+      <c r="H54" s="70"/>
+      <c r="I54" s="70"/>
+      <c r="J54" s="70"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="67" t="s">
+        <v>235</v>
+      </c>
+      <c r="C55" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="67" t="s">
+        <v>251</v>
+      </c>
+      <c r="E55" s="67" t="s">
+        <v>234</v>
+      </c>
+      <c r="F55" s="67" t="s">
+        <v>51</v>
+      </c>
+      <c r="G55" s="67" t="s">
+        <v>236</v>
+      </c>
+      <c r="H55" s="67" t="s">
+        <v>237</v>
+      </c>
+      <c r="I55" s="67" t="s">
+        <v>238</v>
+      </c>
+      <c r="J55" s="67" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="68"/>
+      <c r="B56" s="71" t="s">
+        <v>280</v>
+      </c>
+      <c r="C56" s="70" t="s">
+        <v>278</v>
+      </c>
+      <c r="D56" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="E56" s="70" t="s">
+        <v>281</v>
+      </c>
+      <c r="F56" s="70" t="s">
+        <v>279</v>
+      </c>
+      <c r="G56" s="66" t="s">
+        <v>282</v>
+      </c>
+      <c r="H56" s="60" t="s">
+        <v>254</v>
+      </c>
+      <c r="I56" s="60" t="s">
+        <v>254</v>
+      </c>
+      <c r="J56" s="60" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="68"/>
+      <c r="B57" s="68"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="70"/>
+      <c r="E57" s="70"/>
+      <c r="F57" s="70"/>
+      <c r="G57" s="70"/>
+      <c r="H57" s="68"/>
+      <c r="I57" s="70"/>
+      <c r="J57" s="70"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="58" t="s">
+        <v>283</v>
+      </c>
+      <c r="B58" s="67" t="s">
+        <v>235</v>
+      </c>
+      <c r="C58" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="67"/>
+      <c r="E58" s="70"/>
+      <c r="F58" s="70"/>
+      <c r="G58" s="68"/>
+      <c r="H58" s="70"/>
+      <c r="I58" s="70"/>
+      <c r="J58" s="70"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="70"/>
+      <c r="B59" s="71" t="s">
+        <v>280</v>
+      </c>
+      <c r="C59" s="70" t="s">
+        <v>278</v>
+      </c>
+      <c r="D59" s="70"/>
+      <c r="E59" s="68"/>
+      <c r="F59" s="70"/>
+      <c r="G59" s="70"/>
+      <c r="H59" s="70"/>
+      <c r="I59" s="70"/>
+      <c r="J59" s="70"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="70"/>
+      <c r="B60" s="70"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="70"/>
+      <c r="E60" s="68"/>
+      <c r="F60" s="70"/>
+      <c r="G60" s="70"/>
+      <c r="H60" s="70"/>
+      <c r="I60" s="70"/>
+      <c r="J60" s="70"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="67" t="s">
+        <v>263</v>
+      </c>
+      <c r="B61" s="70"/>
+      <c r="C61" s="70"/>
+      <c r="D61" s="67" t="s">
+        <v>168</v>
+      </c>
+      <c r="E61" s="67" t="s">
+        <v>234</v>
+      </c>
+      <c r="F61" s="67" t="s">
+        <v>51</v>
+      </c>
+      <c r="G61" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="H61" s="67" t="s">
+        <v>236</v>
+      </c>
+      <c r="I61" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="J61" s="70"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="70"/>
+      <c r="B62" s="70"/>
+      <c r="C62" s="70"/>
+      <c r="D62" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="E62" s="70" t="s">
+        <v>281</v>
+      </c>
+      <c r="F62" s="70" t="s">
+        <v>279</v>
+      </c>
+      <c r="G62" s="66" t="s">
+        <v>284</v>
+      </c>
+      <c r="H62" s="66" t="s">
+        <v>285</v>
+      </c>
+      <c r="I62" s="66" t="s">
+        <v>282</v>
+      </c>
+      <c r="J62" s="70"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="66" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.06319444444444" bottom="1.06319444444444" header="0.7875" footer="0.511805555555555"/>
@@ -34399,349 +35513,349 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="72" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="55" t="s">
-        <v>258</v>
-      </c>
-      <c r="E1" s="55" t="s">
-        <v>259</v>
-      </c>
-      <c r="F1" s="55" t="s">
+      <c r="D1" s="72" t="s">
+        <v>287</v>
+      </c>
+      <c r="E1" s="72" t="s">
+        <v>288</v>
+      </c>
+      <c r="F1" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="55" t="s">
-        <v>260</v>
-      </c>
-      <c r="H1" s="55" t="s">
-        <v>261</v>
-      </c>
-      <c r="I1" s="55"/>
+      <c r="G1" s="72" t="s">
+        <v>289</v>
+      </c>
+      <c r="H1" s="72" t="s">
+        <v>290</v>
+      </c>
+      <c r="I1" s="72"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="74" t="s">
         <v>186</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="58" t="s">
-        <v>262</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>263</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>264</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>265</v>
-      </c>
-      <c r="G2" s="57" t="s">
+      <c r="C2" s="75" t="s">
+        <v>291</v>
+      </c>
+      <c r="D2" s="74" t="s">
+        <v>292</v>
+      </c>
+      <c r="E2" s="74" t="s">
+        <v>293</v>
+      </c>
+      <c r="F2" s="74" t="s">
+        <v>294</v>
+      </c>
+      <c r="G2" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="74" t="s">
         <v>213</v>
       </c>
-      <c r="B3" s="59" t="n">
+      <c r="B3" s="76" t="n">
         <v>42625</v>
       </c>
-      <c r="C3" s="58" t="s">
-        <v>266</v>
-      </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57" t="s">
+      <c r="C3" s="75" t="s">
+        <v>295</v>
+      </c>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74" t="s">
         <v>213</v>
       </c>
-      <c r="G3" s="57" t="s">
+      <c r="G3" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="B4" s="59" t="s">
-        <v>267</v>
-      </c>
-      <c r="C4" s="58" t="s">
-        <v>268</v>
-      </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57" t="s">
+      <c r="B4" s="76" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>297</v>
+      </c>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74" t="s">
         <v>181</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="57" t="s">
-        <v>269</v>
-      </c>
-      <c r="B5" s="58" t="s">
-        <v>270</v>
-      </c>
-      <c r="C5" s="58" t="s">
-        <v>271</v>
-      </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57" t="s">
-        <v>272</v>
-      </c>
-      <c r="G5" s="57" t="s">
+      <c r="A5" s="74" t="s">
+        <v>298</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>299</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>300</v>
+      </c>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="G5" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="60" t="n">
+      <c r="B6" s="77" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="58" t="s">
-        <v>273</v>
-      </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57" t="s">
-        <v>272</v>
-      </c>
-      <c r="G6" s="57" t="s">
+      <c r="C6" s="75" t="s">
+        <v>301</v>
+      </c>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74" t="s">
+        <v>248</v>
+      </c>
+      <c r="G6" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="61"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="78"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="57" t="s">
-        <v>274</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>275</v>
-      </c>
-      <c r="C7" s="58" t="s">
+      <c r="A7" s="74" t="s">
+        <v>302</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>303</v>
+      </c>
+      <c r="C7" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57" t="s">
-        <v>274</v>
-      </c>
-      <c r="G7" s="57" t="s">
-        <v>276</v>
-      </c>
-      <c r="H7" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="I7" s="57"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74" t="s">
+        <v>302</v>
+      </c>
+      <c r="G7" s="74" t="s">
+        <v>304</v>
+      </c>
+      <c r="H7" s="74" t="s">
+        <v>241</v>
+      </c>
+      <c r="I7" s="74"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="58" t="s">
-        <v>277</v>
-      </c>
-      <c r="C8" s="58" t="s">
+      <c r="B8" s="75" t="s">
+        <v>305</v>
+      </c>
+      <c r="C8" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57" t="s">
-        <v>277</v>
-      </c>
-      <c r="G8" s="57" t="s">
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74" t="s">
+        <v>305</v>
+      </c>
+      <c r="G8" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="57" t="s">
-        <v>277</v>
-      </c>
-      <c r="B9" s="58" t="s">
-        <v>277</v>
-      </c>
-      <c r="C9" s="58" t="s">
-        <v>278</v>
-      </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57" t="s">
-        <v>277</v>
-      </c>
-      <c r="G9" s="57" t="s">
-        <v>276</v>
-      </c>
-      <c r="H9" s="57" t="s">
-        <v>243</v>
-      </c>
-      <c r="I9" s="57"/>
+      <c r="A9" s="74" t="s">
+        <v>305</v>
+      </c>
+      <c r="B9" s="75" t="s">
+        <v>305</v>
+      </c>
+      <c r="C9" s="75" t="s">
+        <v>306</v>
+      </c>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74" t="s">
+        <v>305</v>
+      </c>
+      <c r="G9" s="74" t="s">
+        <v>304</v>
+      </c>
+      <c r="H9" s="74" t="s">
+        <v>242</v>
+      </c>
+      <c r="I9" s="74"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="57" t="s">
-        <v>279</v>
-      </c>
-      <c r="B10" s="59" t="n">
+      <c r="A10" s="74" t="s">
+        <v>307</v>
+      </c>
+      <c r="B10" s="76" t="n">
         <v>0.480555555555556</v>
       </c>
-      <c r="C10" s="58" t="s">
-        <v>280</v>
-      </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57" t="s">
-        <v>279</v>
-      </c>
-      <c r="G10" s="57" t="s">
+      <c r="C10" s="75" t="s">
+        <v>308</v>
+      </c>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74" t="s">
+        <v>307</v>
+      </c>
+      <c r="G10" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="57" t="s">
-        <v>281</v>
-      </c>
-      <c r="B11" s="58" t="s">
-        <v>282</v>
-      </c>
-      <c r="C11" s="58" t="s">
-        <v>283</v>
-      </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57" t="s">
-        <v>281</v>
-      </c>
-      <c r="G11" s="57" t="s">
+      <c r="A11" s="74" t="s">
+        <v>309</v>
+      </c>
+      <c r="B11" s="75" t="s">
+        <v>310</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>311</v>
+      </c>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74" t="s">
+        <v>309</v>
+      </c>
+      <c r="G11" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="57"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="74"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="74"/>
+      <c r="I12" s="74"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="72" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="56" t="s">
+      <c r="C13" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="55" t="s">
-        <v>258</v>
-      </c>
-      <c r="E13" s="55" t="s">
-        <v>284</v>
-      </c>
-      <c r="F13" s="55" t="s">
-        <v>260</v>
-      </c>
-      <c r="G13" s="55" t="s">
-        <v>260</v>
-      </c>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
+      <c r="D13" s="72" t="s">
+        <v>287</v>
+      </c>
+      <c r="E13" s="72" t="s">
+        <v>312</v>
+      </c>
+      <c r="F13" s="72" t="s">
+        <v>289</v>
+      </c>
+      <c r="G13" s="72" t="s">
+        <v>289</v>
+      </c>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="60" t="n">
+      <c r="B14" s="77" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="58" t="s">
-        <v>285</v>
-      </c>
-      <c r="D14" s="57" t="s">
-        <v>286</v>
-      </c>
-      <c r="E14" s="57" t="s">
-        <v>287</v>
-      </c>
-      <c r="F14" s="57" t="s">
-        <v>265</v>
-      </c>
-      <c r="G14" s="57" t="s">
+      <c r="C14" s="75" t="s">
+        <v>313</v>
+      </c>
+      <c r="D14" s="74" t="s">
+        <v>314</v>
+      </c>
+      <c r="E14" s="74" t="s">
+        <v>315</v>
+      </c>
+      <c r="F14" s="74" t="s">
+        <v>294</v>
+      </c>
+      <c r="G14" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -34765,13 +35879,13 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="58" t="s">
-        <v>275</v>
-      </c>
-      <c r="F16" s="58" t="s">
+      <c r="E16" s="75" t="s">
+        <v>303</v>
+      </c>
+      <c r="F16" s="75" t="s">
         <v>160</v>
       </c>
-      <c r="G16" s="58"/>
+      <c r="G16" s="75"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -34783,13 +35897,13 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="57" t="s">
+      <c r="E17" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="57" t="s">
-        <v>288</v>
-      </c>
-      <c r="G17" s="57"/>
+      <c r="F17" s="74" t="s">
+        <v>316</v>
+      </c>
+      <c r="G17" s="74"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -34812,21 +35926,21 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="4" t="s">
-        <v>289</v>
+        <v>317</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="4" t="s">
-        <v>290</v>
+        <v>318</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="4" t="s">
-        <v>291</v>
+        <v>319</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -34838,17 +35952,17 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="4" t="s">
-        <v>292</v>
+        <v>320</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="4" t="s">
-        <v>292</v>
+        <v>320</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="4" t="s">
-        <v>292</v>
+        <v>320</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -34859,32 +35973,32 @@
         <v>58</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>293</v>
+        <v>321</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>293</v>
+        <v>321</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>58</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>294</v>
+        <v>322</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>293</v>
+        <v>321</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
         <v>58</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>295</v>
+        <v>323</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>293</v>
+        <v>321</v>
       </c>
       <c r="L21" s="3"/>
     </row>
@@ -34937,32 +36051,32 @@
         <v>64</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>296</v>
+        <v>324</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>297</v>
+        <v>325</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>64</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>297</v>
+        <v>325</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
         <v>64</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>299</v>
+        <v>327</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>297</v>
+        <v>325</v>
       </c>
       <c r="L24" s="3"/>
     </row>
@@ -34971,7 +36085,7 @@
         <v>64</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>300</v>
+        <v>328</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>64</v>
@@ -34981,7 +36095,7 @@
         <v>64</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>301</v>
+        <v>329</v>
       </c>
       <c r="G25" s="15" t="n">
         <v>1919</v>
@@ -34991,7 +36105,7 @@
         <v>64</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>302</v>
+        <v>330</v>
       </c>
       <c r="K25" s="15" t="n">
         <v>1919</v>
@@ -35003,32 +36117,32 @@
         <v>65</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>65</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>294</v>
+        <v>322</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3" t="s">
         <v>65</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>295</v>
+        <v>323</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>303</v>
+        <v>331</v>
       </c>
       <c r="L26" s="3"/>
     </row>
@@ -35059,32 +36173,32 @@
         <v>68</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>304</v>
+        <v>332</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>304</v>
+        <v>332</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>304</v>
+        <v>332</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3" t="s">
         <v>68</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>299</v>
+        <v>327</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>304</v>
+        <v>332</v>
       </c>
       <c r="L28" s="3"/>
     </row>
@@ -35093,7 +36207,7 @@
         <v>70</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>305</v>
+        <v>333</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>70</v>
@@ -35105,7 +36219,7 @@
         <v>70</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="G29" s="14" t="n">
         <v>2</v>
@@ -35115,7 +36229,7 @@
         <v>70</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>299</v>
+        <v>327</v>
       </c>
       <c r="K29" s="14" t="n">
         <v>2</v>
@@ -35152,7 +36266,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -35168,7 +36282,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>306</v>
+        <v>334</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -35189,7 +36303,7 @@
         <v>58</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>307</v>
+        <v>335</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -35197,7 +36311,7 @@
         <v>58</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>307</v>
+        <v>335</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -35229,7 +36343,7 @@
         <v>62</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>308</v>
+        <v>336</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -35237,7 +36351,7 @@
         <v>62</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>308</v>
+        <v>336</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -35251,7 +36365,7 @@
         <v>64</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>309</v>
+        <v>337</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -35259,7 +36373,7 @@
         <v>64</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>309</v>
+        <v>337</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -35273,7 +36387,7 @@
         <v>65</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -35281,7 +36395,7 @@
         <v>65</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -35295,7 +36409,7 @@
         <v>68</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>311</v>
+        <v>339</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -35303,7 +36417,7 @@
         <v>68</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>311</v>
+        <v>339</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -35317,7 +36431,7 @@
         <v>70</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>305</v>
+        <v>333</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>37</v>
@@ -35327,13 +36441,13 @@
         <v>70</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>305</v>
+        <v>333</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>312</v>
+        <v>340</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>313</v>
+        <v>341</v>
       </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
@@ -35345,17 +36459,17 @@
         <v>86</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>314</v>
+        <v>342</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>315</v>
+        <v>343</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3" t="s">
         <v>88</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>316</v>
+        <v>344</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -35367,19 +36481,19 @@
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
-        <v>317</v>
+        <v>345</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3" t="s">
-        <v>318</v>
+        <v>346</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>319</v>
+        <v>347</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3" t="s">
-        <v>320</v>
+        <v>348</v>
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
@@ -35389,21 +36503,21 @@
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
       <c r="B43" s="3" t="s">
-        <v>321</v>
+        <v>349</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3" t="s">
-        <v>322</v>
+        <v>350</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>324</v>
+        <v>352</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>320</v>
+        <v>348</v>
       </c>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
@@ -35458,9 +36572,9 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="9.14"/>
@@ -35469,7 +36583,7 @@
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
-        <v>325</v>
+        <v>353</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -35482,17 +36596,17 @@
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>326</v>
+        <v>354</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>326</v>
+        <v>354</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="3" t="s">
-        <v>327</v>
+        <v>355</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>327</v>
+        <v>355</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -35500,18 +36614,18 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
-      <c r="B3" s="62" t="s">
-        <v>328</v>
-      </c>
-      <c r="C3" s="62" t="s">
-        <v>328</v>
-      </c>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62" t="s">
-        <v>328</v>
-      </c>
-      <c r="F3" s="62" t="s">
-        <v>328</v>
+      <c r="B3" s="79" t="s">
+        <v>356</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>356</v>
+      </c>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79" t="s">
+        <v>356</v>
+      </c>
+      <c r="F3" s="79" t="s">
+        <v>356</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -35519,17 +36633,17 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62" t="s">
+      <c r="D4" s="79"/>
+      <c r="E4" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="79" t="s">
         <v>34</v>
       </c>
       <c r="G4" s="3"/>
@@ -35539,17 +36653,17 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>329</v>
+        <v>357</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>330</v>
+        <v>358</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>331</v>
+        <v>359</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>332</v>
+        <v>360</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -35559,12 +36673,12 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>333</v>
+        <v>361</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>333</v>
+        <v>361</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -35574,12 +36688,12 @@
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="11" t="s">
-        <v>334</v>
+        <v>362</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="11" t="s">
-        <v>334</v>
+        <v>362</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -35589,17 +36703,17 @@
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>336</v>
+        <v>363</v>
+      </c>
+      <c r="D8" s="80" t="s">
+        <v>364</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G8" s="63" t="s">
-        <v>336</v>
+        <v>363</v>
+      </c>
+      <c r="G8" s="80" t="s">
+        <v>364</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -35609,12 +36723,12 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="11" t="s">
-        <v>337</v>
+        <v>365</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11" t="s">
-        <v>337</v>
+        <v>365</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -35623,13 +36737,13 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="64" t="s">
-        <v>338</v>
+      <c r="D10" s="81" t="s">
+        <v>366</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="64" t="s">
-        <v>338</v>
+      <c r="G10" s="81" t="s">
+        <v>366</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -35638,13 +36752,13 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="64" t="s">
-        <v>339</v>
+      <c r="D11" s="81" t="s">
+        <v>367</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="64" t="s">
-        <v>339</v>
+      <c r="G11" s="81" t="s">
+        <v>367</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -35653,13 +36767,13 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="64" t="s">
-        <v>340</v>
+      <c r="D12" s="81" t="s">
+        <v>368</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="64" t="s">
-        <v>340</v>
+      <c r="G12" s="81" t="s">
+        <v>368</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -35667,17 +36781,17 @@
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>341</v>
+        <v>369</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>341</v>
+        <v>369</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>341</v>
+        <v>369</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>341</v>
+        <v>369</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -35686,17 +36800,17 @@
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>342</v>
+        <v>370</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>342</v>
+        <v>370</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>342</v>
+        <v>370</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>342</v>
+        <v>370</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -35705,38 +36819,38 @@
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>343</v>
+        <v>371</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>343</v>
+        <v>371</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>343</v>
+        <v>371</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>343</v>
+        <v>371</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>344</v>
+        <v>372</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
-      <c r="B16" s="62" t="s">
-        <v>345</v>
-      </c>
-      <c r="C16" s="62" t="s">
-        <v>345</v>
+      <c r="B16" s="79" t="s">
+        <v>373</v>
+      </c>
+      <c r="C16" s="79" t="s">
+        <v>373</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="62" t="s">
-        <v>345</v>
-      </c>
-      <c r="F16" s="62" t="s">
-        <v>345</v>
+      <c r="E16" s="79" t="s">
+        <v>373</v>
+      </c>
+      <c r="F16" s="79" t="s">
+        <v>373</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -35745,17 +36859,17 @@
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>346</v>
+        <v>374</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>346</v>
+        <v>374</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>347</v>
+        <v>375</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>347</v>
+        <v>375</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -35764,17 +36878,17 @@
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
       <c r="B18" s="28" t="s">
-        <v>348</v>
+        <v>376</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>348</v>
+        <v>376</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="28" t="s">
-        <v>348</v>
+        <v>376</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>348</v>
+        <v>376</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -35822,51 +36936,51 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="65"/>
-      <c r="B1" s="66" t="s">
-        <v>349</v>
-      </c>
-      <c r="C1" s="66" t="s">
-        <v>350</v>
-      </c>
-      <c r="D1" s="66" t="s">
-        <v>351</v>
-      </c>
-      <c r="E1" s="66" t="s">
-        <v>352</v>
+      <c r="A1" s="82"/>
+      <c r="B1" s="83" t="s">
+        <v>377</v>
+      </c>
+      <c r="C1" s="83" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1" s="83" t="s">
+        <v>379</v>
+      </c>
+      <c r="E1" s="83" t="s">
+        <v>380</v>
       </c>
       <c r="F1" s="3"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
     </row>
     <row r="2" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="66" t="s">
-        <v>353</v>
+      <c r="A2" s="83" t="s">
+        <v>381</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>354</v>
+        <v>382</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>354</v>
+        <v>382</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>355</v>
+        <v>383</v>
       </c>
       <c r="E2" s="50" t="s">
-        <v>356</v>
+        <v>384</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="66" t="s">
-        <v>357</v>
+      <c r="A3" s="83" t="s">
+        <v>385</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>358</v>
+        <v>386</v>
       </c>
       <c r="C3" s="50" t="s">
         <v>180</v>
@@ -35878,9 +36992,9 @@
         <v>180</v>
       </c>
       <c r="F3" s="3"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
framework uses its own logger instead the one from waitress
</commit_message>
<xml_diff>
--- a/doc/design.xlsx
+++ b/doc/design.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="591">
   <si>
     <t xml:space="preserve">component</t>
   </si>
@@ -1494,6 +1494,15 @@
     <t xml:space="preserve">update first 1000 records (partial)</t>
   </si>
   <si>
+    <t xml:space="preserve">/var on slow disk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/var=/ HDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/var=/ SSD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Source</t>
   </si>
   <si>
@@ -1826,12 +1835,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY/DD/MM"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY\ HH:MM"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
     <numFmt numFmtId="169" formatCode="0%"/>
     <numFmt numFmtId="170" formatCode="@"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="44">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2148,6 +2157,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i val="true"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -2282,7 +2299,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2681,6 +2698,10 @@
     </xf>
     <xf numFmtId="164" fontId="42" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="41" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -32474,27 +32495,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32504,26 +32527,34 @@
       <c r="B1" s="93" t="s">
         <v>460</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="93" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93" t="s">
+        <v>460</v>
+      </c>
+      <c r="F1" s="93"/>
+      <c r="G1" s="94" t="s">
         <v>461</v>
-      </c>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94" t="s">
-        <v>462</v>
-      </c>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94" t="s">
-        <v>463</v>
       </c>
       <c r="H1" s="94"/>
       <c r="I1" s="94" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J1" s="94"/>
       <c r="K1" s="94" t="s">
+        <v>463</v>
+      </c>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94" t="s">
+        <v>463</v>
+      </c>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94" t="s">
         <v>464</v>
       </c>
-      <c r="L1" s="94"/>
+      <c r="P1" s="94"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="92" t="s">
@@ -32532,26 +32563,34 @@
       <c r="B2" s="93" t="s">
         <v>466</v>
       </c>
-      <c r="C2" s="94" t="s">
+      <c r="C2" s="93" t="s">
+        <v>466</v>
+      </c>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93" t="s">
+        <v>466</v>
+      </c>
+      <c r="F2" s="93"/>
+      <c r="G2" s="94" t="s">
         <v>467</v>
-      </c>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94" t="s">
-        <v>468</v>
-      </c>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94" t="s">
-        <v>469</v>
       </c>
       <c r="H2" s="94"/>
       <c r="I2" s="94" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="J2" s="94"/>
       <c r="K2" s="94" t="s">
+        <v>469</v>
+      </c>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94" t="s">
+        <v>470</v>
+      </c>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94" t="s">
         <v>468</v>
       </c>
-      <c r="L2" s="94"/>
+      <c r="P2" s="94"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="92" t="s">
@@ -32590,6 +32629,18 @@
       <c r="L3" s="93" t="s">
         <v>472</v>
       </c>
+      <c r="M3" s="93" t="s">
+        <v>345</v>
+      </c>
+      <c r="N3" s="93" t="s">
+        <v>472</v>
+      </c>
+      <c r="O3" s="93" t="s">
+        <v>345</v>
+      </c>
+      <c r="P3" s="93" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="87" t="s">
@@ -32598,39 +32649,53 @@
       <c r="B4" s="95" t="n">
         <v>0.016424</v>
       </c>
-      <c r="C4" s="96" t="n">
+      <c r="C4" s="95" t="n">
+        <v>0.001563</v>
+      </c>
+      <c r="D4" s="96" t="n">
+        <f aca="false">C4/B4</f>
+        <v>0.0951656113005358</v>
+      </c>
+      <c r="E4" s="95" t="n">
+        <v>0.000453</v>
+      </c>
+      <c r="F4" s="96" t="n">
+        <f aca="false">E4/B4</f>
+        <v>0.0275815879201169</v>
+      </c>
+      <c r="G4" s="97" t="n">
         <v>0.048995</v>
       </c>
-      <c r="D4" s="97" t="n">
-        <f aca="false">C4/B4</f>
+      <c r="H4" s="96" t="n">
+        <f aca="false">G4/B4</f>
         <v>2.98313443740867</v>
       </c>
-      <c r="E4" s="95" t="n">
+      <c r="I4" s="95" t="n">
         <v>0.102591</v>
-      </c>
-      <c r="F4" s="98" t="n">
-        <f aca="false">E4/B4</f>
-        <v>6.24640769605456</v>
-      </c>
-      <c r="G4" s="95" t="n">
-        <v>0.047733</v>
-      </c>
-      <c r="H4" s="98" t="n">
-        <f aca="false">G4/B4</f>
-        <v>2.90629566488066</v>
-      </c>
-      <c r="I4" s="87" t="n">
-        <v>0.017323</v>
       </c>
       <c r="J4" s="98" t="n">
         <f aca="false">I4/B4</f>
-        <v>1.05473697028738</v>
+        <v>6.24640769605456</v>
       </c>
       <c r="K4" s="95" t="n">
-        <v>0.076974</v>
+        <v>0.047733</v>
       </c>
       <c r="L4" s="98" t="n">
         <f aca="false">K4/B4</f>
+        <v>2.90629566488066</v>
+      </c>
+      <c r="M4" s="87" t="n">
+        <v>0.017323</v>
+      </c>
+      <c r="N4" s="98" t="n">
+        <f aca="false">M4/B4</f>
+        <v>1.05473697028738</v>
+      </c>
+      <c r="O4" s="95" t="n">
+        <v>0.076974</v>
+      </c>
+      <c r="P4" s="98" t="n">
+        <f aca="false">O4/B4</f>
         <v>4.68667803214808</v>
       </c>
     </row>
@@ -32641,39 +32706,53 @@
       <c r="B5" s="95" t="n">
         <v>0.017911</v>
       </c>
-      <c r="C5" s="96" t="n">
+      <c r="C5" s="95" t="n">
+        <v>0.001212</v>
+      </c>
+      <c r="D5" s="96" t="n">
+        <f aca="false">C5/B5</f>
+        <v>0.0676679135726648</v>
+      </c>
+      <c r="E5" s="95" t="n">
+        <v>0.000548</v>
+      </c>
+      <c r="F5" s="96" t="n">
+        <f aca="false">E5/B5</f>
+        <v>0.0305957232985316</v>
+      </c>
+      <c r="G5" s="97" t="n">
         <v>0.008847</v>
       </c>
-      <c r="D5" s="97" t="n">
-        <f aca="false">C5/B5</f>
+      <c r="H5" s="96" t="n">
+        <f aca="false">G5/B5</f>
         <v>0.493942270113338</v>
       </c>
-      <c r="E5" s="95" t="n">
+      <c r="I5" s="95" t="n">
         <v>0.224636</v>
-      </c>
-      <c r="F5" s="98" t="n">
-        <f aca="false">E5/B5</f>
-        <v>12.5417899614762</v>
-      </c>
-      <c r="G5" s="95" t="n">
-        <v>0.118356</v>
-      </c>
-      <c r="H5" s="98" t="n">
-        <f aca="false">G5/B5</f>
-        <v>6.60800625314053</v>
-      </c>
-      <c r="I5" s="87" t="n">
-        <v>0.022906</v>
       </c>
       <c r="J5" s="98" t="n">
         <f aca="false">I5/B5</f>
-        <v>1.27887890123388</v>
+        <v>12.5417899614762</v>
       </c>
       <c r="K5" s="95" t="n">
-        <v>2.457824</v>
+        <v>0.118356</v>
       </c>
       <c r="L5" s="98" t="n">
         <f aca="false">K5/B5</f>
+        <v>6.60800625314053</v>
+      </c>
+      <c r="M5" s="87" t="n">
+        <v>0.022906</v>
+      </c>
+      <c r="N5" s="98" t="n">
+        <f aca="false">M5/B5</f>
+        <v>1.27887890123388</v>
+      </c>
+      <c r="O5" s="95" t="n">
+        <v>2.457824</v>
+      </c>
+      <c r="P5" s="98" t="n">
+        <f aca="false">O5/B5</f>
         <v>137.224275584836</v>
       </c>
     </row>
@@ -32684,39 +32763,53 @@
       <c r="B6" s="95" t="n">
         <v>0.062072</v>
       </c>
-      <c r="C6" s="96" t="n">
+      <c r="C6" s="97" t="n">
+        <v>0.00076</v>
+      </c>
+      <c r="D6" s="96" t="n">
+        <f aca="false">C6/B6</f>
+        <v>0.0122438458564248</v>
+      </c>
+      <c r="E6" s="97" t="n">
+        <v>0.00037</v>
+      </c>
+      <c r="F6" s="96" t="n">
+        <f aca="false">E6/B6</f>
+        <v>0.00596081969325944</v>
+      </c>
+      <c r="G6" s="97" t="n">
         <v>0.079314</v>
       </c>
-      <c r="D6" s="97" t="n">
-        <f aca="false">C6/B6</f>
+      <c r="H6" s="96" t="n">
+        <f aca="false">G6/B6</f>
         <v>1.27777419770589</v>
       </c>
-      <c r="E6" s="95" t="n">
+      <c r="I6" s="95" t="n">
         <v>0.106703</v>
-      </c>
-      <c r="F6" s="98" t="n">
-        <f aca="false">E6/B6</f>
-        <v>1.71901984791855</v>
-      </c>
-      <c r="G6" s="95" t="n">
-        <v>0.102644</v>
-      </c>
-      <c r="H6" s="98" t="n">
-        <f aca="false">G6/B6</f>
-        <v>1.65362804485114</v>
-      </c>
-      <c r="I6" s="87" t="n">
-        <v>0.052501</v>
       </c>
       <c r="J6" s="98" t="n">
         <f aca="false">I6/B6</f>
-        <v>0.845808093826524</v>
+        <v>1.71901984791855</v>
       </c>
       <c r="K6" s="95" t="n">
-        <v>2.548866</v>
+        <v>0.102644</v>
       </c>
       <c r="L6" s="98" t="n">
         <f aca="false">K6/B6</f>
+        <v>1.65362804485114</v>
+      </c>
+      <c r="M6" s="87" t="n">
+        <v>0.052501</v>
+      </c>
+      <c r="N6" s="98" t="n">
+        <f aca="false">M6/B6</f>
+        <v>0.845808093826524</v>
+      </c>
+      <c r="O6" s="95" t="n">
+        <v>2.548866</v>
+      </c>
+      <c r="P6" s="98" t="n">
+        <f aca="false">O6/B6</f>
         <v>41.0630558061606</v>
       </c>
     </row>
@@ -32727,39 +32820,53 @@
       <c r="B7" s="95" t="n">
         <v>0.027084</v>
       </c>
-      <c r="C7" s="96" t="n">
+      <c r="C7" s="95" t="n">
+        <v>0.000668</v>
+      </c>
+      <c r="D7" s="96" t="n">
+        <f aca="false">C7/B7</f>
+        <v>0.0246640082705656</v>
+      </c>
+      <c r="E7" s="95" t="n">
+        <v>0.000314</v>
+      </c>
+      <c r="F7" s="96" t="n">
+        <f aca="false">E7/B7</f>
+        <v>0.0115935607738886</v>
+      </c>
+      <c r="G7" s="97" t="n">
         <v>0.012179</v>
       </c>
-      <c r="D7" s="97" t="n">
-        <f aca="false">C7/B7</f>
+      <c r="H7" s="96" t="n">
+        <f aca="false">G7/B7</f>
         <v>0.449675084920987</v>
       </c>
-      <c r="E7" s="95" t="n">
+      <c r="I7" s="95" t="n">
         <v>0.150609</v>
-      </c>
-      <c r="F7" s="98" t="n">
-        <f aca="false">E7/B7</f>
-        <v>5.56081081081081</v>
-      </c>
-      <c r="G7" s="95" t="n">
-        <v>0.056508</v>
-      </c>
-      <c r="H7" s="98" t="n">
-        <f aca="false">G7/B7</f>
-        <v>2.08639787328312</v>
-      </c>
-      <c r="I7" s="87" t="n">
-        <v>0.033761</v>
       </c>
       <c r="J7" s="98" t="n">
         <f aca="false">I7/B7</f>
-        <v>1.24652931620145</v>
+        <v>5.56081081081081</v>
       </c>
       <c r="K7" s="95" t="n">
-        <v>2.274458</v>
+        <v>0.056508</v>
       </c>
       <c r="L7" s="98" t="n">
         <f aca="false">K7/B7</f>
+        <v>2.08639787328312</v>
+      </c>
+      <c r="M7" s="87" t="n">
+        <v>0.033761</v>
+      </c>
+      <c r="N7" s="98" t="n">
+        <f aca="false">M7/B7</f>
+        <v>1.24652931620145</v>
+      </c>
+      <c r="O7" s="95" t="n">
+        <v>2.274458</v>
+      </c>
+      <c r="P7" s="98" t="n">
+        <f aca="false">O7/B7</f>
         <v>83.9779205434943</v>
       </c>
     </row>
@@ -32771,30 +32878,44 @@
         <v>0.137918</v>
       </c>
       <c r="C8" s="95" t="n">
+        <v>0.000694</v>
+      </c>
+      <c r="D8" s="96" t="n">
+        <f aca="false">C8/B8</f>
+        <v>0.0050319755216868</v>
+      </c>
+      <c r="E8" s="95" t="n">
+        <v>0.000297</v>
+      </c>
+      <c r="F8" s="96" t="n">
+        <f aca="false">E8/B8</f>
+        <v>0.00215345350135588</v>
+      </c>
+      <c r="G8" s="95" t="n">
         <v>0.045261</v>
       </c>
-      <c r="D8" s="97" t="n">
-        <f aca="false">C8/B8</f>
+      <c r="H8" s="96" t="n">
+        <f aca="false">G8/B8</f>
         <v>0.328173262373294</v>
       </c>
-      <c r="E8" s="95" t="n">
+      <c r="I8" s="95" t="n">
         <v>0.343385</v>
-      </c>
-      <c r="F8" s="98" t="n">
-        <f aca="false">E8/B8</f>
-        <v>2.48977653388245</v>
-      </c>
-      <c r="G8" s="99"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="87" t="n">
-        <v>0.172413</v>
       </c>
       <c r="J8" s="98" t="n">
         <f aca="false">I8/B8</f>
-        <v>1.25011238562044</v>
+        <v>2.48977653388245</v>
       </c>
       <c r="K8" s="99"/>
       <c r="L8" s="99"/>
+      <c r="M8" s="87" t="n">
+        <v>0.172413</v>
+      </c>
+      <c r="N8" s="98" t="n">
+        <f aca="false">M8/B8</f>
+        <v>1.25011238562044</v>
+      </c>
+      <c r="O8" s="99"/>
+      <c r="P8" s="99"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="87" t="s">
@@ -32804,35 +32925,49 @@
         <v>0.360714</v>
       </c>
       <c r="C9" s="95" t="n">
+        <v>0.000681</v>
+      </c>
+      <c r="D9" s="96" t="n">
+        <f aca="false">C9/B9</f>
+        <v>0.0018879222874632</v>
+      </c>
+      <c r="E9" s="95" t="n">
+        <v>0.000271</v>
+      </c>
+      <c r="F9" s="96" t="n">
+        <f aca="false">E9/B9</f>
+        <v>0.000751287723792256</v>
+      </c>
+      <c r="G9" s="95" t="n">
         <v>0.148961</v>
       </c>
-      <c r="D9" s="97" t="n">
-        <f aca="false">C9/B9</f>
+      <c r="H9" s="96" t="n">
+        <f aca="false">G9/B9</f>
         <v>0.412961515217042</v>
       </c>
-      <c r="E9" s="95" t="n">
+      <c r="I9" s="95" t="n">
         <v>31.425577</v>
-      </c>
-      <c r="F9" s="98" t="n">
-        <f aca="false">E9/B9</f>
-        <v>87.1204804914697</v>
-      </c>
-      <c r="G9" s="95" t="n">
-        <v>1.901056</v>
-      </c>
-      <c r="H9" s="98" t="n">
-        <f aca="false">G9/B9</f>
-        <v>5.27025843188787</v>
-      </c>
-      <c r="I9" s="87" t="n">
-        <v>1.688972</v>
       </c>
       <c r="J9" s="98" t="n">
         <f aca="false">I9/B9</f>
+        <v>87.1204804914697</v>
+      </c>
+      <c r="K9" s="95" t="n">
+        <v>1.901056</v>
+      </c>
+      <c r="L9" s="98" t="n">
+        <f aca="false">K9/B9</f>
+        <v>5.27025843188787</v>
+      </c>
+      <c r="M9" s="87" t="n">
+        <v>1.688972</v>
+      </c>
+      <c r="N9" s="98" t="n">
+        <f aca="false">M9/B9</f>
         <v>4.6823023226157</v>
       </c>
-      <c r="K9" s="99"/>
-      <c r="L9" s="99"/>
+      <c r="O9" s="99"/>
+      <c r="P9" s="99"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="87" t="s">
@@ -32841,19 +32976,46 @@
       <c r="B10" s="95" t="n">
         <v>0.410004</v>
       </c>
+      <c r="C10" s="95" t="n">
+        <v>0.00067</v>
+      </c>
+      <c r="D10" s="96" t="n">
+        <f aca="false">C10/B10</f>
+        <v>0.00163413039872782</v>
+      </c>
+      <c r="E10" s="95" t="n">
+        <v>0.000268</v>
+      </c>
+      <c r="F10" s="96" t="n">
+        <f aca="false">E10/B10</f>
+        <v>0.000653652159491127</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="87" t="s">
+        <v>480</v>
+      </c>
+      <c r="C12" s="87" t="s">
+        <v>481</v>
+      </c>
+      <c r="D12" s="100"/>
+      <c r="E12" s="87" t="s">
+        <v>482</v>
+      </c>
+      <c r="F12" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -32898,527 +33060,527 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="100" t="s">
-        <v>480</v>
-      </c>
-      <c r="B1" s="101" t="s">
+      <c r="A1" s="101" t="s">
+        <v>483</v>
+      </c>
+      <c r="B1" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="101" t="s">
+      <c r="C1" s="102" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="102" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="102" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="101" t="s">
+      <c r="F1" s="102" t="s">
         <v>185</v>
       </c>
-      <c r="G1" s="101" t="s">
-        <v>481</v>
-      </c>
-      <c r="H1" s="101" t="s">
-        <v>482</v>
-      </c>
-      <c r="I1" s="101" t="s">
-        <v>483</v>
-      </c>
-      <c r="J1" s="101" t="s">
+      <c r="G1" s="102" t="s">
         <v>484</v>
       </c>
-      <c r="K1" s="101" t="s">
+      <c r="H1" s="102" t="s">
         <v>485</v>
       </c>
-      <c r="L1" s="101" t="s">
+      <c r="I1" s="102" t="s">
         <v>486</v>
       </c>
-      <c r="M1" s="101" t="s">
+      <c r="J1" s="102" t="s">
+        <v>487</v>
+      </c>
+      <c r="K1" s="102" t="s">
+        <v>488</v>
+      </c>
+      <c r="L1" s="102" t="s">
+        <v>489</v>
+      </c>
+      <c r="M1" s="102" t="s">
         <v>343</v>
       </c>
-      <c r="N1" s="101" t="s">
-        <v>487</v>
-      </c>
-      <c r="O1" s="101" t="s">
-        <v>488</v>
-      </c>
-      <c r="P1" s="101" t="s">
-        <v>489</v>
-      </c>
-      <c r="Q1" s="101" t="s">
+      <c r="N1" s="102" t="s">
         <v>490</v>
+      </c>
+      <c r="O1" s="102" t="s">
+        <v>491</v>
+      </c>
+      <c r="P1" s="102" t="s">
+        <v>492</v>
+      </c>
+      <c r="Q1" s="102" t="s">
+        <v>493</v>
       </c>
       <c r="R1" s="87"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="102"/>
-      <c r="B2" s="103" t="n">
+      <c r="A2" s="103"/>
+      <c r="B2" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="103" t="s">
-        <v>491</v>
-      </c>
-      <c r="D2" s="104" t="s">
-        <v>492</v>
-      </c>
-      <c r="E2" s="104" t="s">
-        <v>493</v>
-      </c>
-      <c r="F2" s="103" t="s">
+      <c r="C2" s="104" t="s">
         <v>494</v>
       </c>
-      <c r="G2" s="103" t="s">
+      <c r="D2" s="105" t="s">
         <v>495</v>
       </c>
-      <c r="H2" s="103" t="s">
+      <c r="E2" s="105" t="s">
         <v>496</v>
       </c>
-      <c r="I2" s="103" t="n">
+      <c r="F2" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="G2" s="104" t="s">
+        <v>498</v>
+      </c>
+      <c r="H2" s="104" t="s">
+        <v>499</v>
+      </c>
+      <c r="I2" s="104" t="n">
         <v>57</v>
       </c>
-      <c r="J2" s="103" t="n">
+      <c r="J2" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="K2" s="104" t="s">
-        <v>497</v>
-      </c>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103" t="s">
-        <v>498</v>
-      </c>
-      <c r="N2" s="103" t="n">
+      <c r="K2" s="105" t="s">
+        <v>500</v>
+      </c>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104" t="s">
+        <v>501</v>
+      </c>
+      <c r="N2" s="104" t="n">
         <v>111</v>
       </c>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103" t="s">
-        <v>499</v>
-      </c>
-      <c r="Q2" s="103" t="n">
+      <c r="O2" s="104"/>
+      <c r="P2" s="104" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q2" s="104" t="n">
         <v>6970</v>
       </c>
       <c r="R2" s="87"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="102"/>
-      <c r="B3" s="103" t="n">
+      <c r="A3" s="103"/>
+      <c r="B3" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="103" t="s">
-        <v>491</v>
-      </c>
-      <c r="D3" s="104" t="s">
-        <v>500</v>
-      </c>
-      <c r="E3" s="104" t="s">
-        <v>501</v>
-      </c>
-      <c r="F3" s="103" t="s">
+      <c r="C3" s="104" t="s">
         <v>494</v>
       </c>
-      <c r="G3" s="103" t="s">
-        <v>495</v>
-      </c>
-      <c r="H3" s="103" t="s">
-        <v>502</v>
-      </c>
-      <c r="I3" s="103" t="n">
+      <c r="D3" s="105" t="s">
+        <v>503</v>
+      </c>
+      <c r="E3" s="105" t="s">
+        <v>504</v>
+      </c>
+      <c r="F3" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="G3" s="104" t="s">
+        <v>498</v>
+      </c>
+      <c r="H3" s="104" t="s">
+        <v>505</v>
+      </c>
+      <c r="I3" s="104" t="n">
         <v>13</v>
       </c>
-      <c r="J3" s="103" t="n">
+      <c r="J3" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="104" t="s">
-        <v>503</v>
-      </c>
-      <c r="L3" s="103"/>
-      <c r="M3" s="103" t="s">
-        <v>504</v>
-      </c>
-      <c r="N3" s="103"/>
-      <c r="O3" s="103" t="n">
+      <c r="K3" s="105" t="s">
+        <v>506</v>
+      </c>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104" t="s">
+        <v>507</v>
+      </c>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104" t="n">
         <v>111</v>
       </c>
-      <c r="P3" s="103" t="s">
-        <v>505</v>
-      </c>
-      <c r="Q3" s="103" t="n">
+      <c r="P3" s="104" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q3" s="104" t="n">
         <v>6973</v>
       </c>
       <c r="R3" s="87"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="102"/>
-      <c r="B4" s="103" t="n">
+      <c r="A4" s="103"/>
+      <c r="B4" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="103" t="s">
-        <v>491</v>
-      </c>
-      <c r="D4" s="104" t="s">
-        <v>506</v>
-      </c>
-      <c r="E4" s="104" t="s">
-        <v>507</v>
-      </c>
-      <c r="F4" s="103" t="s">
+      <c r="C4" s="104" t="s">
         <v>494</v>
       </c>
-      <c r="G4" s="103" t="s">
-        <v>508</v>
-      </c>
-      <c r="H4" s="103" t="s">
+      <c r="D4" s="105" t="s">
         <v>509</v>
       </c>
-      <c r="I4" s="103" t="n">
+      <c r="E4" s="105" t="s">
+        <v>510</v>
+      </c>
+      <c r="F4" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="G4" s="104" t="s">
+        <v>511</v>
+      </c>
+      <c r="H4" s="104" t="s">
+        <v>512</v>
+      </c>
+      <c r="I4" s="104" t="n">
         <v>125</v>
       </c>
-      <c r="J4" s="103" t="n">
+      <c r="J4" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="K4" s="104" t="s">
-        <v>510</v>
-      </c>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103" t="s">
-        <v>511</v>
-      </c>
-      <c r="N4" s="103" t="n">
+      <c r="K4" s="105" t="s">
+        <v>513</v>
+      </c>
+      <c r="L4" s="104"/>
+      <c r="M4" s="104" t="s">
+        <v>514</v>
+      </c>
+      <c r="N4" s="104" t="n">
         <v>222</v>
       </c>
-      <c r="O4" s="103"/>
-      <c r="P4" s="103" t="s">
-        <v>512</v>
-      </c>
-      <c r="Q4" s="103" t="n">
+      <c r="O4" s="104"/>
+      <c r="P4" s="104" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q4" s="104" t="n">
         <v>6969</v>
       </c>
       <c r="R4" s="87"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="102"/>
-      <c r="B5" s="103" t="n">
+      <c r="A5" s="103"/>
+      <c r="B5" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="103" t="s">
-        <v>491</v>
-      </c>
-      <c r="D5" s="104" t="s">
-        <v>513</v>
-      </c>
-      <c r="E5" s="104" t="s">
-        <v>514</v>
-      </c>
-      <c r="F5" s="103" t="s">
+      <c r="C5" s="104" t="s">
         <v>494</v>
       </c>
-      <c r="G5" s="103" t="s">
-        <v>515</v>
-      </c>
-      <c r="H5" s="103" t="s">
+      <c r="D5" s="105" t="s">
         <v>516</v>
       </c>
-      <c r="I5" s="103" t="n">
+      <c r="E5" s="105" t="s">
+        <v>517</v>
+      </c>
+      <c r="F5" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="G5" s="104" t="s">
+        <v>518</v>
+      </c>
+      <c r="H5" s="104" t="s">
+        <v>519</v>
+      </c>
+      <c r="I5" s="104" t="n">
         <v>57</v>
       </c>
-      <c r="J5" s="103" t="n">
+      <c r="J5" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="K5" s="104" t="s">
-        <v>517</v>
-      </c>
-      <c r="L5" s="103"/>
-      <c r="M5" s="103" t="s">
-        <v>518</v>
-      </c>
-      <c r="N5" s="103"/>
-      <c r="O5" s="103" t="n">
+      <c r="K5" s="105" t="s">
+        <v>520</v>
+      </c>
+      <c r="L5" s="104"/>
+      <c r="M5" s="104" t="s">
+        <v>521</v>
+      </c>
+      <c r="N5" s="104"/>
+      <c r="O5" s="104" t="n">
         <v>222</v>
       </c>
-      <c r="P5" s="103" t="s">
-        <v>519</v>
-      </c>
-      <c r="Q5" s="103" t="n">
+      <c r="P5" s="104" t="s">
+        <v>522</v>
+      </c>
+      <c r="Q5" s="104" t="n">
         <v>6962</v>
       </c>
       <c r="R5" s="87"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103" t="n">
+      <c r="A6" s="103"/>
+      <c r="B6" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="103" t="s">
-        <v>491</v>
-      </c>
-      <c r="D6" s="104" t="s">
-        <v>520</v>
-      </c>
-      <c r="E6" s="104" t="s">
-        <v>521</v>
-      </c>
-      <c r="F6" s="103" t="s">
+      <c r="C6" s="104" t="s">
         <v>494</v>
       </c>
-      <c r="G6" s="103" t="s">
-        <v>508</v>
-      </c>
-      <c r="H6" s="103" t="s">
-        <v>522</v>
-      </c>
-      <c r="I6" s="103" t="n">
+      <c r="D6" s="105" t="s">
+        <v>523</v>
+      </c>
+      <c r="E6" s="105" t="s">
+        <v>524</v>
+      </c>
+      <c r="F6" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="G6" s="104" t="s">
+        <v>511</v>
+      </c>
+      <c r="H6" s="104" t="s">
+        <v>525</v>
+      </c>
+      <c r="I6" s="104" t="n">
         <v>163</v>
       </c>
-      <c r="J6" s="103" t="n">
+      <c r="J6" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="K6" s="104" t="s">
-        <v>523</v>
-      </c>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103" t="s">
-        <v>524</v>
-      </c>
-      <c r="N6" s="103" t="n">
+      <c r="K6" s="105" t="s">
+        <v>526</v>
+      </c>
+      <c r="L6" s="104"/>
+      <c r="M6" s="104" t="s">
+        <v>527</v>
+      </c>
+      <c r="N6" s="104" t="n">
         <v>333</v>
       </c>
-      <c r="O6" s="103"/>
-      <c r="P6" s="103" t="s">
-        <v>525</v>
-      </c>
-      <c r="Q6" s="103" t="n">
+      <c r="O6" s="104"/>
+      <c r="P6" s="104" t="s">
+        <v>528</v>
+      </c>
+      <c r="Q6" s="104" t="n">
         <v>6968</v>
       </c>
       <c r="R6" s="87"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="102"/>
-      <c r="B7" s="103" t="n">
+      <c r="A7" s="103"/>
+      <c r="B7" s="104" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="103" t="s">
-        <v>491</v>
-      </c>
-      <c r="D7" s="104" t="s">
-        <v>526</v>
-      </c>
-      <c r="E7" s="104" t="s">
-        <v>527</v>
-      </c>
-      <c r="F7" s="103" t="s">
+      <c r="C7" s="104" t="s">
         <v>494</v>
       </c>
-      <c r="G7" s="103" t="s">
-        <v>528</v>
-      </c>
-      <c r="H7" s="103" t="s">
+      <c r="D7" s="105" t="s">
         <v>529</v>
       </c>
-      <c r="I7" s="103" t="n">
+      <c r="E7" s="105" t="s">
+        <v>530</v>
+      </c>
+      <c r="F7" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="G7" s="104" t="s">
+        <v>531</v>
+      </c>
+      <c r="H7" s="104" t="s">
+        <v>532</v>
+      </c>
+      <c r="I7" s="104" t="n">
         <v>11</v>
       </c>
-      <c r="J7" s="103" t="n">
+      <c r="J7" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="K7" s="104" t="s">
-        <v>530</v>
-      </c>
-      <c r="L7" s="103"/>
-      <c r="M7" s="103" t="s">
-        <v>531</v>
-      </c>
-      <c r="N7" s="103"/>
-      <c r="O7" s="103" t="n">
+      <c r="K7" s="105" t="s">
+        <v>533</v>
+      </c>
+      <c r="L7" s="104"/>
+      <c r="M7" s="104" t="s">
+        <v>534</v>
+      </c>
+      <c r="N7" s="104"/>
+      <c r="O7" s="104" t="n">
         <v>333</v>
       </c>
-      <c r="P7" s="103" t="s">
-        <v>532</v>
-      </c>
-      <c r="Q7" s="103" t="n">
+      <c r="P7" s="104" t="s">
+        <v>535</v>
+      </c>
+      <c r="Q7" s="104" t="n">
         <v>6956</v>
       </c>
       <c r="R7" s="87"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="102"/>
-      <c r="B8" s="103" t="n">
+      <c r="A8" s="103"/>
+      <c r="B8" s="104" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="103" t="s">
-        <v>491</v>
-      </c>
-      <c r="D8" s="104" t="s">
-        <v>533</v>
-      </c>
-      <c r="E8" s="104" t="s">
-        <v>534</v>
-      </c>
-      <c r="F8" s="103" t="s">
+      <c r="C8" s="104" t="s">
         <v>494</v>
       </c>
-      <c r="G8" s="103" t="s">
-        <v>535</v>
-      </c>
-      <c r="H8" s="103" t="s">
+      <c r="D8" s="105" t="s">
         <v>536</v>
       </c>
-      <c r="I8" s="103" t="n">
+      <c r="E8" s="105" t="s">
+        <v>537</v>
+      </c>
+      <c r="F8" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="G8" s="104" t="s">
+        <v>538</v>
+      </c>
+      <c r="H8" s="104" t="s">
+        <v>539</v>
+      </c>
+      <c r="I8" s="104" t="n">
         <v>54</v>
       </c>
-      <c r="J8" s="103" t="n">
+      <c r="J8" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="K8" s="104" t="s">
-        <v>537</v>
-      </c>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103" t="s">
-        <v>538</v>
-      </c>
-      <c r="N8" s="103"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="103" t="s">
-        <v>539</v>
-      </c>
-      <c r="Q8" s="103" t="n">
+      <c r="K8" s="105" t="s">
+        <v>540</v>
+      </c>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104" t="s">
+        <v>541</v>
+      </c>
+      <c r="N8" s="104"/>
+      <c r="O8" s="104"/>
+      <c r="P8" s="104" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q8" s="104" t="n">
         <v>6963</v>
       </c>
       <c r="R8" s="87"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="102"/>
-      <c r="B9" s="103" t="n">
+      <c r="A9" s="103"/>
+      <c r="B9" s="104" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="103" t="s">
-        <v>491</v>
-      </c>
-      <c r="D9" s="104" t="s">
-        <v>540</v>
-      </c>
-      <c r="E9" s="104" t="s">
-        <v>541</v>
-      </c>
-      <c r="F9" s="103" t="s">
+      <c r="C9" s="104" t="s">
         <v>494</v>
       </c>
-      <c r="G9" s="103" t="s">
-        <v>528</v>
-      </c>
-      <c r="H9" s="103" t="s">
-        <v>542</v>
-      </c>
-      <c r="I9" s="103" t="n">
+      <c r="D9" s="105" t="s">
+        <v>543</v>
+      </c>
+      <c r="E9" s="105" t="s">
+        <v>544</v>
+      </c>
+      <c r="F9" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="G9" s="104" t="s">
+        <v>531</v>
+      </c>
+      <c r="H9" s="104" t="s">
+        <v>545</v>
+      </c>
+      <c r="I9" s="104" t="n">
         <v>44</v>
       </c>
-      <c r="J9" s="103" t="n">
+      <c r="J9" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="K9" s="104" t="s">
-        <v>543</v>
-      </c>
-      <c r="L9" s="103"/>
-      <c r="M9" s="103" t="s">
-        <v>544</v>
-      </c>
-      <c r="N9" s="103"/>
-      <c r="O9" s="103"/>
-      <c r="P9" s="103" t="s">
-        <v>545</v>
-      </c>
-      <c r="Q9" s="103" t="n">
+      <c r="K9" s="105" t="s">
+        <v>546</v>
+      </c>
+      <c r="L9" s="104"/>
+      <c r="M9" s="104" t="s">
+        <v>547</v>
+      </c>
+      <c r="N9" s="104"/>
+      <c r="O9" s="104"/>
+      <c r="P9" s="104" t="s">
+        <v>548</v>
+      </c>
+      <c r="Q9" s="104" t="n">
         <v>6957</v>
       </c>
       <c r="R9" s="87"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="102"/>
-      <c r="B10" s="103" t="n">
+      <c r="A10" s="103"/>
+      <c r="B10" s="104" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="103" t="s">
-        <v>491</v>
-      </c>
-      <c r="D10" s="104" t="s">
-        <v>546</v>
-      </c>
-      <c r="E10" s="104" t="s">
-        <v>547</v>
-      </c>
-      <c r="F10" s="103" t="s">
+      <c r="C10" s="104" t="s">
         <v>494</v>
       </c>
-      <c r="G10" s="103" t="s">
-        <v>495</v>
-      </c>
-      <c r="H10" s="103" t="s">
-        <v>548</v>
-      </c>
-      <c r="I10" s="103" t="n">
+      <c r="D10" s="105" t="s">
+        <v>549</v>
+      </c>
+      <c r="E10" s="105" t="s">
+        <v>550</v>
+      </c>
+      <c r="F10" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="G10" s="104" t="s">
+        <v>498</v>
+      </c>
+      <c r="H10" s="104" t="s">
+        <v>551</v>
+      </c>
+      <c r="I10" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="J10" s="103" t="n">
+      <c r="J10" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="K10" s="104" t="s">
-        <v>549</v>
-      </c>
-      <c r="L10" s="103"/>
-      <c r="M10" s="103" t="s">
-        <v>550</v>
-      </c>
-      <c r="N10" s="103"/>
-      <c r="O10" s="103"/>
-      <c r="P10" s="103" t="s">
-        <v>551</v>
-      </c>
-      <c r="Q10" s="103" t="n">
+      <c r="K10" s="105" t="s">
+        <v>552</v>
+      </c>
+      <c r="L10" s="104"/>
+      <c r="M10" s="104" t="s">
+        <v>553</v>
+      </c>
+      <c r="N10" s="104"/>
+      <c r="O10" s="104"/>
+      <c r="P10" s="104" t="s">
+        <v>554</v>
+      </c>
+      <c r="Q10" s="104" t="n">
         <v>6971</v>
       </c>
       <c r="R10" s="87"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="102"/>
-      <c r="B11" s="103" t="n">
+      <c r="A11" s="103"/>
+      <c r="B11" s="104" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="103" t="s">
-        <v>491</v>
-      </c>
-      <c r="D11" s="104" t="s">
-        <v>552</v>
-      </c>
-      <c r="E11" s="104" t="s">
-        <v>501</v>
-      </c>
-      <c r="F11" s="103" t="s">
+      <c r="C11" s="104" t="s">
         <v>494</v>
       </c>
-      <c r="G11" s="103" t="s">
-        <v>495</v>
-      </c>
-      <c r="H11" s="103" t="s">
-        <v>553</v>
-      </c>
-      <c r="I11" s="103" t="n">
+      <c r="D11" s="105" t="s">
+        <v>555</v>
+      </c>
+      <c r="E11" s="105" t="s">
+        <v>504</v>
+      </c>
+      <c r="F11" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="G11" s="104" t="s">
+        <v>498</v>
+      </c>
+      <c r="H11" s="104" t="s">
+        <v>556</v>
+      </c>
+      <c r="I11" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="J11" s="103" t="n">
+      <c r="J11" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="K11" s="104" t="s">
-        <v>554</v>
-      </c>
-      <c r="L11" s="103"/>
-      <c r="M11" s="103" t="s">
-        <v>555</v>
-      </c>
-      <c r="N11" s="103"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="103" t="s">
-        <v>556</v>
-      </c>
-      <c r="Q11" s="103" t="n">
+      <c r="K11" s="105" t="s">
+        <v>557</v>
+      </c>
+      <c r="L11" s="104"/>
+      <c r="M11" s="104" t="s">
+        <v>558</v>
+      </c>
+      <c r="N11" s="104"/>
+      <c r="O11" s="104"/>
+      <c r="P11" s="104" t="s">
+        <v>559</v>
+      </c>
+      <c r="Q11" s="104" t="n">
         <v>6972</v>
       </c>
       <c r="R11" s="87"/>
@@ -33444,28 +33606,28 @@
       <c r="R12" s="87"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="100" t="s">
-        <v>557</v>
-      </c>
-      <c r="B13" s="101" t="s">
+      <c r="A13" s="101" t="s">
+        <v>560</v>
+      </c>
+      <c r="B13" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="101" t="s">
-        <v>558</v>
-      </c>
-      <c r="D13" s="101" t="s">
+      <c r="C13" s="102" t="s">
+        <v>561</v>
+      </c>
+      <c r="D13" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="100" t="s">
-        <v>559</v>
-      </c>
-      <c r="G13" s="101" t="s">
+      <c r="F13" s="101" t="s">
+        <v>562</v>
+      </c>
+      <c r="G13" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="H13" s="101" t="s">
-        <v>560</v>
-      </c>
-      <c r="I13" s="101" t="s">
+      <c r="H13" s="102" t="s">
+        <v>563</v>
+      </c>
+      <c r="I13" s="102" t="s">
         <v>35</v>
       </c>
       <c r="L13" s="87"/>
@@ -33477,25 +33639,25 @@
       <c r="R13" s="87"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="103"/>
-      <c r="B14" s="103" t="n">
+      <c r="A14" s="104"/>
+      <c r="B14" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="C14" s="103" t="n">
+      <c r="C14" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="D14" s="103" t="s">
-        <v>561</v>
-      </c>
-      <c r="F14" s="103"/>
-      <c r="G14" s="103" t="n">
+      <c r="D14" s="104" t="s">
+        <v>564</v>
+      </c>
+      <c r="F14" s="104"/>
+      <c r="G14" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="H14" s="103" t="n">
+      <c r="H14" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="I14" s="103" t="s">
-        <v>561</v>
+      <c r="I14" s="104" t="s">
+        <v>564</v>
       </c>
       <c r="L14" s="87"/>
       <c r="M14" s="87"/>
@@ -33506,25 +33668,25 @@
       <c r="R14" s="87"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="103"/>
-      <c r="B15" s="103" t="n">
+      <c r="A15" s="104"/>
+      <c r="B15" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="C15" s="103" t="n">
+      <c r="C15" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="D15" s="103" t="s">
-        <v>562</v>
-      </c>
-      <c r="F15" s="103"/>
-      <c r="G15" s="103" t="n">
+      <c r="D15" s="104" t="s">
+        <v>565</v>
+      </c>
+      <c r="F15" s="104"/>
+      <c r="G15" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="H15" s="103" t="n">
+      <c r="H15" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="I15" s="103" t="s">
-        <v>562</v>
+      <c r="I15" s="104" t="s">
+        <v>565</v>
       </c>
       <c r="L15" s="87"/>
       <c r="M15" s="87"/>
@@ -33535,25 +33697,25 @@
       <c r="R15" s="87"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="103"/>
-      <c r="B16" s="103" t="n">
+      <c r="A16" s="104"/>
+      <c r="B16" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="C16" s="103" t="n">
+      <c r="C16" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="103" t="s">
-        <v>563</v>
-      </c>
-      <c r="F16" s="103"/>
-      <c r="G16" s="103" t="n">
+      <c r="D16" s="104" t="s">
+        <v>566</v>
+      </c>
+      <c r="F16" s="104"/>
+      <c r="G16" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="H16" s="103" t="n">
+      <c r="H16" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="I16" s="103" t="s">
-        <v>563</v>
+      <c r="I16" s="104" t="s">
+        <v>566</v>
       </c>
       <c r="L16" s="87"/>
       <c r="M16" s="87"/>
@@ -33564,25 +33726,25 @@
       <c r="R16" s="87"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="103"/>
-      <c r="B17" s="103" t="n">
+      <c r="A17" s="104"/>
+      <c r="B17" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="103" t="n">
+      <c r="C17" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="D17" s="103" t="s">
-        <v>564</v>
-      </c>
-      <c r="F17" s="103"/>
-      <c r="G17" s="103" t="n">
+      <c r="D17" s="104" t="s">
+        <v>567</v>
+      </c>
+      <c r="F17" s="104"/>
+      <c r="G17" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="H17" s="103" t="n">
+      <c r="H17" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="I17" s="103" t="s">
-        <v>564</v>
+      <c r="I17" s="104" t="s">
+        <v>567</v>
       </c>
       <c r="L17" s="87"/>
       <c r="M17" s="87"/>
@@ -33593,25 +33755,25 @@
       <c r="R17" s="87"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="103"/>
-      <c r="B18" s="103" t="n">
+      <c r="A18" s="104"/>
+      <c r="B18" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="C18" s="103" t="n">
+      <c r="C18" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="D18" s="103" t="s">
-        <v>565</v>
-      </c>
-      <c r="F18" s="103"/>
-      <c r="G18" s="103" t="n">
+      <c r="D18" s="104" t="s">
+        <v>568</v>
+      </c>
+      <c r="F18" s="104"/>
+      <c r="G18" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="H18" s="103" t="n">
+      <c r="H18" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="I18" s="103" t="s">
-        <v>565</v>
+      <c r="I18" s="104" t="s">
+        <v>568</v>
       </c>
       <c r="L18" s="87"/>
       <c r="M18" s="87"/>
@@ -33622,25 +33784,25 @@
       <c r="R18" s="87"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="103"/>
-      <c r="B19" s="103" t="n">
+      <c r="A19" s="104"/>
+      <c r="B19" s="104" t="n">
         <v>5</v>
       </c>
-      <c r="C19" s="103" t="n">
+      <c r="C19" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="D19" s="103" t="s">
-        <v>566</v>
-      </c>
-      <c r="F19" s="103"/>
-      <c r="G19" s="103" t="n">
+      <c r="D19" s="104" t="s">
+        <v>569</v>
+      </c>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104" t="n">
         <v>5</v>
       </c>
-      <c r="H19" s="103" t="n">
+      <c r="H19" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="I19" s="103" t="s">
-        <v>566</v>
+      <c r="I19" s="104" t="s">
+        <v>569</v>
       </c>
       <c r="L19" s="87"/>
       <c r="M19" s="87"/>
@@ -33651,25 +33813,25 @@
       <c r="R19" s="87"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="103"/>
-      <c r="B20" s="103" t="n">
+      <c r="A20" s="104"/>
+      <c r="B20" s="104" t="n">
         <v>6</v>
       </c>
-      <c r="C20" s="103" t="n">
+      <c r="C20" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="D20" s="103" t="s">
-        <v>567</v>
-      </c>
-      <c r="F20" s="103"/>
-      <c r="G20" s="103" t="n">
+      <c r="D20" s="104" t="s">
+        <v>570</v>
+      </c>
+      <c r="F20" s="104"/>
+      <c r="G20" s="104" t="n">
         <v>6</v>
       </c>
-      <c r="H20" s="103" t="n">
+      <c r="H20" s="104" t="n">
         <v>6</v>
       </c>
-      <c r="I20" s="103" t="s">
-        <v>567</v>
+      <c r="I20" s="104" t="s">
+        <v>570</v>
       </c>
       <c r="L20" s="87"/>
       <c r="M20" s="87"/>
@@ -33680,25 +33842,25 @@
       <c r="R20" s="87"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="103"/>
-      <c r="B21" s="103" t="n">
+      <c r="A21" s="104"/>
+      <c r="B21" s="104" t="n">
         <v>7</v>
       </c>
-      <c r="C21" s="103" t="n">
+      <c r="C21" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="D21" s="103" t="s">
-        <v>568</v>
-      </c>
-      <c r="F21" s="103"/>
-      <c r="G21" s="103" t="n">
+      <c r="D21" s="104" t="s">
+        <v>571</v>
+      </c>
+      <c r="F21" s="104"/>
+      <c r="G21" s="104" t="n">
         <v>7</v>
       </c>
-      <c r="H21" s="103" t="n">
+      <c r="H21" s="104" t="n">
         <v>6</v>
       </c>
-      <c r="I21" s="103" t="s">
-        <v>568</v>
+      <c r="I21" s="104" t="s">
+        <v>571</v>
       </c>
       <c r="L21" s="87"/>
       <c r="M21" s="87"/>
@@ -33709,25 +33871,25 @@
       <c r="R21" s="87"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="103"/>
-      <c r="B22" s="103" t="n">
+      <c r="A22" s="104"/>
+      <c r="B22" s="104" t="n">
         <v>8</v>
       </c>
-      <c r="C22" s="103" t="n">
+      <c r="C22" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="D22" s="103" t="s">
-        <v>569</v>
-      </c>
-      <c r="F22" s="103"/>
-      <c r="G22" s="103" t="n">
+      <c r="D22" s="104" t="s">
+        <v>572</v>
+      </c>
+      <c r="F22" s="104"/>
+      <c r="G22" s="104" t="n">
         <v>8</v>
       </c>
-      <c r="H22" s="103" t="n">
+      <c r="H22" s="104" t="n">
         <v>6</v>
       </c>
-      <c r="I22" s="103" t="s">
-        <v>569</v>
+      <c r="I22" s="104" t="s">
+        <v>572</v>
       </c>
       <c r="L22" s="87"/>
       <c r="M22" s="87"/>
@@ -33738,25 +33900,25 @@
       <c r="R22" s="87"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="103"/>
-      <c r="B23" s="103" t="n">
+      <c r="A23" s="104"/>
+      <c r="B23" s="104" t="n">
         <v>9</v>
       </c>
-      <c r="C23" s="103" t="n">
+      <c r="C23" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="D23" s="103" t="s">
-        <v>570</v>
-      </c>
-      <c r="F23" s="103"/>
-      <c r="G23" s="103" t="n">
+      <c r="D23" s="104" t="s">
+        <v>573</v>
+      </c>
+      <c r="F23" s="104"/>
+      <c r="G23" s="104" t="n">
         <v>9</v>
       </c>
-      <c r="H23" s="103" t="n">
+      <c r="H23" s="104" t="n">
         <v>6</v>
       </c>
-      <c r="I23" s="103" t="s">
-        <v>570</v>
+      <c r="I23" s="104" t="s">
+        <v>573</v>
       </c>
       <c r="L23" s="87"/>
       <c r="M23" s="87"/>
@@ -33787,19 +33949,19 @@
       <c r="R24" s="87"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="100" t="s">
-        <v>571</v>
-      </c>
-      <c r="B25" s="101" t="s">
+      <c r="A25" s="101" t="s">
+        <v>574</v>
+      </c>
+      <c r="B25" s="102" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="101" t="s">
-        <v>572</v>
-      </c>
-      <c r="D25" s="101" t="s">
+      <c r="C25" s="102" t="s">
+        <v>575</v>
+      </c>
+      <c r="D25" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="101" t="s">
+      <c r="E25" s="102" t="s">
         <v>109</v>
       </c>
       <c r="G25" s="87"/>
@@ -33816,153 +33978,153 @@
       <c r="R25" s="87"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="103"/>
-      <c r="B26" s="103" t="n">
+      <c r="A26" s="104"/>
+      <c r="B26" s="104" t="n">
         <v>0</v>
       </c>
-      <c r="C26" s="103" t="n">
+      <c r="C26" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="103" t="s">
-        <v>573</v>
-      </c>
-      <c r="E26" s="103" t="s">
-        <v>574</v>
+      <c r="D26" s="104" t="s">
+        <v>576</v>
+      </c>
+      <c r="E26" s="104" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="103"/>
-      <c r="B27" s="103" t="n">
+      <c r="A27" s="104"/>
+      <c r="B27" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="103" t="n">
+      <c r="C27" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="103" t="s">
-        <v>575</v>
-      </c>
-      <c r="E27" s="103" t="s">
-        <v>576</v>
+      <c r="D27" s="104" t="s">
+        <v>578</v>
+      </c>
+      <c r="E27" s="104" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="103"/>
-      <c r="B28" s="103" t="n">
+      <c r="A28" s="104"/>
+      <c r="B28" s="104" t="n">
         <v>2</v>
       </c>
-      <c r="C28" s="103" t="n">
+      <c r="C28" s="104" t="n">
         <v>1</v>
       </c>
-      <c r="D28" s="103" t="s">
-        <v>577</v>
-      </c>
-      <c r="E28" s="103" t="s">
-        <v>578</v>
+      <c r="D28" s="104" t="s">
+        <v>580</v>
+      </c>
+      <c r="E28" s="104" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="103"/>
-      <c r="B29" s="103" t="n">
+      <c r="A29" s="104"/>
+      <c r="B29" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="C29" s="103" t="n">
+      <c r="C29" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="D29" s="103" t="s">
-        <v>573</v>
-      </c>
-      <c r="E29" s="103" t="s">
-        <v>574</v>
+      <c r="D29" s="104" t="s">
+        <v>576</v>
+      </c>
+      <c r="E29" s="104" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="103"/>
-      <c r="B30" s="103" t="n">
+      <c r="A30" s="104"/>
+      <c r="B30" s="104" t="n">
         <v>4</v>
       </c>
-      <c r="C30" s="103" t="n">
+      <c r="C30" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="D30" s="103" t="s">
-        <v>577</v>
-      </c>
-      <c r="E30" s="103" t="s">
-        <v>578</v>
+      <c r="D30" s="104" t="s">
+        <v>580</v>
+      </c>
+      <c r="E30" s="104" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="103"/>
-      <c r="B31" s="103" t="n">
+      <c r="A31" s="104"/>
+      <c r="B31" s="104" t="n">
         <v>5</v>
       </c>
-      <c r="C31" s="103" t="n">
+      <c r="C31" s="104" t="n">
         <v>3</v>
       </c>
-      <c r="D31" s="103" t="s">
-        <v>575</v>
-      </c>
-      <c r="E31" s="103" t="s">
-        <v>576</v>
+      <c r="D31" s="104" t="s">
+        <v>578</v>
+      </c>
+      <c r="E31" s="104" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="103"/>
-      <c r="B32" s="103" t="n">
+      <c r="A32" s="104"/>
+      <c r="B32" s="104" t="n">
         <v>6</v>
       </c>
-      <c r="C32" s="103" t="n">
+      <c r="C32" s="104" t="n">
         <v>5</v>
       </c>
-      <c r="D32" s="103" t="s">
-        <v>573</v>
-      </c>
-      <c r="E32" s="103" t="s">
-        <v>574</v>
+      <c r="D32" s="104" t="s">
+        <v>576</v>
+      </c>
+      <c r="E32" s="104" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="103"/>
-      <c r="B33" s="103" t="n">
+      <c r="A33" s="104"/>
+      <c r="B33" s="104" t="n">
         <v>7</v>
       </c>
-      <c r="C33" s="103" t="n">
+      <c r="C33" s="104" t="n">
         <v>5</v>
       </c>
-      <c r="D33" s="103" t="s">
-        <v>577</v>
-      </c>
-      <c r="E33" s="103" t="s">
-        <v>578</v>
+      <c r="D33" s="104" t="s">
+        <v>580</v>
+      </c>
+      <c r="E33" s="104" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="103"/>
-      <c r="B34" s="103" t="n">
+      <c r="A34" s="104"/>
+      <c r="B34" s="104" t="n">
         <v>8</v>
       </c>
-      <c r="C34" s="103" t="n">
+      <c r="C34" s="104" t="n">
         <v>5</v>
       </c>
-      <c r="D34" s="103" t="s">
-        <v>579</v>
-      </c>
-      <c r="E34" s="103" t="s">
-        <v>580</v>
+      <c r="D34" s="104" t="s">
+        <v>582</v>
+      </c>
+      <c r="E34" s="104" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="103"/>
-      <c r="B35" s="103" t="n">
+      <c r="A35" s="104"/>
+      <c r="B35" s="104" t="n">
         <v>9</v>
       </c>
-      <c r="C35" s="103" t="n">
+      <c r="C35" s="104" t="n">
         <v>5</v>
       </c>
-      <c r="D35" s="103" t="s">
-        <v>575</v>
-      </c>
-      <c r="E35" s="103" t="s">
-        <v>576</v>
+      <c r="D35" s="104" t="s">
+        <v>578</v>
+      </c>
+      <c r="E35" s="104" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33977,7 +34139,7 @@
       <c r="L37" s="87"/>
       <c r="M37" s="87"/>
       <c r="N37" s="87" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -33992,7 +34154,7 @@
       <c r="L38" s="87"/>
       <c r="M38" s="87"/>
       <c r="N38" s="87" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34007,7 +34169,7 @@
       <c r="L39" s="87"/>
       <c r="M39" s="87"/>
       <c r="N39" s="87" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34022,7 +34184,7 @@
       <c r="L40" s="87"/>
       <c r="M40" s="87"/>
       <c r="N40" s="87" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34052,7 +34214,7 @@
       <c r="L42" s="87"/>
       <c r="M42" s="87"/>
       <c r="N42" s="87" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34067,7 +34229,7 @@
       <c r="L43" s="87"/>
       <c r="M43" s="87"/>
       <c r="N43" s="87" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34082,7 +34244,7 @@
       <c r="L44" s="87"/>
       <c r="M44" s="87"/>
       <c r="N44" s="87" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34097,7 +34259,7 @@
       <c r="L45" s="87"/>
       <c r="M45" s="87"/>
       <c r="N45" s="87" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -34112,7 +34274,7 @@
       <c r="L46" s="87"/>
       <c r="M46" s="87"/>
       <c r="N46" s="87" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>